<commit_message>
Update with Power Rankings
</commit_message>
<xml_diff>
--- a/Power Rankings.xlsx
+++ b/Power Rankings.xlsx
@@ -3607,8 +3607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3777,7 +3777,9 @@
       <c r="I3" s="36">
         <v>90.7</v>
       </c>
-      <c r="J3" s="36"/>
+      <c r="J3" s="36">
+        <v>93.7</v>
+      </c>
       <c r="K3" s="36"/>
       <c r="L3" s="36"/>
       <c r="M3" s="36"/>
@@ -3785,11 +3787,11 @@
       <c r="O3" s="8"/>
       <c r="P3" s="12">
         <f>SUM(C3:O3)</f>
-        <v>813.4</v>
+        <v>907.1</v>
       </c>
       <c r="Q3" s="12">
         <f>AVERAGE(C3:O3)</f>
-        <v>116.2</v>
+        <v>113.3875</v>
       </c>
       <c r="R3" s="13">
         <f>MAX(C3:O3)</f>
@@ -3801,7 +3803,7 @@
       </c>
       <c r="T3" s="13">
         <f>STDEV(C3:O3)</f>
-        <v>12.724517017684306</v>
+        <v>14.214925506060826</v>
       </c>
       <c r="W3" s="52">
         <f>IF(C3="","",RANK(C3,$C$3:$C$18,1))</f>
@@ -3831,9 +3833,9 @@
         <f>IF(I3="","",RANK(I3,$I$3:$I$18,1))</f>
         <v>7</v>
       </c>
-      <c r="AD3" s="53" t="str">
+      <c r="AD3" s="53">
         <f>IF(J3="","",RANK(J3,$J$3:$J$18,1))</f>
-        <v/>
+        <v>5</v>
       </c>
       <c r="AE3" s="53" t="str">
         <f>IF(K3="","",RANK(K3,$K$3:$K$18,1))</f>
@@ -3857,7 +3859,7 @@
       </c>
       <c r="AJ3" s="42">
         <f>SUM(W3:AI3)</f>
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3888,7 +3890,9 @@
       <c r="I4" s="34">
         <v>57.9</v>
       </c>
-      <c r="J4" s="34"/>
+      <c r="J4" s="34">
+        <v>81.5</v>
+      </c>
       <c r="K4" s="34"/>
       <c r="L4" s="34"/>
       <c r="M4" s="34"/>
@@ -3896,11 +3900,11 @@
       <c r="O4" s="9"/>
       <c r="P4" s="14">
         <f t="shared" ref="P4:P18" si="0">SUM(C4:O4)</f>
-        <v>623</v>
+        <v>704.5</v>
       </c>
       <c r="Q4" s="14">
         <f t="shared" ref="Q4:Q18" si="1">AVERAGE(C4:O4)</f>
-        <v>89</v>
+        <v>88.0625</v>
       </c>
       <c r="R4" s="15">
         <f t="shared" ref="R4:R18" si="2">MAX(C4:O4)</f>
@@ -3912,7 +3916,7 @@
       </c>
       <c r="T4" s="15">
         <f t="shared" ref="T4:T18" si="4">STDEV(C4:O4)</f>
-        <v>27.013268344772115</v>
+        <v>25.149605932726441</v>
       </c>
       <c r="W4" s="55">
         <f t="shared" ref="W4:W18" si="5">IF(C4="","",RANK(C4,$C$3:$C$18,1))</f>
@@ -3942,9 +3946,9 @@
         <f t="shared" ref="AC4:AC18" si="11">IF(I4="","",RANK(I4,$I$3:$I$18,1))</f>
         <v>1</v>
       </c>
-      <c r="AD4" s="56" t="str">
+      <c r="AD4" s="56">
         <f t="shared" ref="AD4:AD18" si="12">IF(J4="","",RANK(J4,$J$3:$J$18,1))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AE4" s="56" t="str">
         <f t="shared" ref="AE4:AE18" si="13">IF(K4="","",RANK(K4,$K$3:$K$18,1))</f>
@@ -3968,7 +3972,7 @@
       </c>
       <c r="AJ4" s="43">
         <f t="shared" ref="AJ4:AJ18" si="18">SUM(W4:AI4)</f>
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3999,7 +4003,9 @@
       <c r="I5" s="36">
         <v>58.1</v>
       </c>
-      <c r="J5" s="36"/>
+      <c r="J5" s="36">
+        <v>106.7</v>
+      </c>
       <c r="K5" s="36"/>
       <c r="L5" s="36"/>
       <c r="M5" s="36"/>
@@ -4007,15 +4013,15 @@
       <c r="O5" s="8"/>
       <c r="P5" s="16">
         <f t="shared" si="0"/>
-        <v>559.40000000000009</v>
+        <v>666.10000000000014</v>
       </c>
       <c r="Q5" s="16">
         <f t="shared" si="1"/>
-        <v>79.914285714285725</v>
+        <v>83.262500000000017</v>
       </c>
       <c r="R5" s="17">
         <f t="shared" si="2"/>
-        <v>101.2</v>
+        <v>106.7</v>
       </c>
       <c r="S5" s="17">
         <f t="shared" si="3"/>
@@ -4023,7 +4029,7 @@
       </c>
       <c r="T5" s="17">
         <f t="shared" si="4"/>
-        <v>15.205857267451005</v>
+        <v>16.966768991177918</v>
       </c>
       <c r="W5" s="55">
         <f t="shared" si="5"/>
@@ -4053,9 +4059,9 @@
         <f t="shared" si="11"/>
         <v>2</v>
       </c>
-      <c r="AD5" s="56" t="str">
+      <c r="AD5" s="56">
         <f t="shared" si="12"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="AE5" s="56" t="str">
         <f t="shared" si="13"/>
@@ -4079,7 +4085,7 @@
       </c>
       <c r="AJ5" s="43">
         <f t="shared" si="18"/>
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4110,7 +4116,9 @@
       <c r="I6" s="35">
         <v>83.2</v>
       </c>
-      <c r="J6" s="36"/>
+      <c r="J6" s="36">
+        <v>119.2</v>
+      </c>
       <c r="K6" s="36"/>
       <c r="L6" s="34"/>
       <c r="M6" s="34"/>
@@ -4118,11 +4126,11 @@
       <c r="O6" s="9"/>
       <c r="P6" s="14">
         <f t="shared" si="0"/>
-        <v>662.1</v>
+        <v>781.30000000000007</v>
       </c>
       <c r="Q6" s="14">
         <f t="shared" si="1"/>
-        <v>94.585714285714289</v>
+        <v>97.662500000000009</v>
       </c>
       <c r="R6" s="15">
         <f t="shared" si="2"/>
@@ -4134,7 +4142,7 @@
       </c>
       <c r="T6" s="15">
         <f t="shared" si="4"/>
-        <v>16.225641083526625</v>
+        <v>17.360705836539488</v>
       </c>
       <c r="W6" s="55">
         <f t="shared" si="5"/>
@@ -4164,9 +4172,9 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-      <c r="AD6" s="56" t="str">
+      <c r="AD6" s="56">
         <f t="shared" si="12"/>
-        <v/>
+        <v>14</v>
       </c>
       <c r="AE6" s="56" t="str">
         <f t="shared" si="13"/>
@@ -4190,7 +4198,7 @@
       </c>
       <c r="AJ6" s="43">
         <f t="shared" si="18"/>
-        <v>45</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4221,7 +4229,9 @@
       <c r="I7" s="33">
         <v>66.099999999999994</v>
       </c>
-      <c r="J7" s="34"/>
+      <c r="J7" s="34">
+        <v>117.6</v>
+      </c>
       <c r="K7" s="34"/>
       <c r="L7" s="36"/>
       <c r="M7" s="36"/>
@@ -4229,11 +4239,11 @@
       <c r="O7" s="8"/>
       <c r="P7" s="16">
         <f t="shared" si="0"/>
-        <v>650.00000000000011</v>
+        <v>767.60000000000014</v>
       </c>
       <c r="Q7" s="16">
         <f t="shared" si="1"/>
-        <v>92.857142857142875</v>
+        <v>95.950000000000017</v>
       </c>
       <c r="R7" s="17">
         <f t="shared" si="2"/>
@@ -4245,7 +4255,7 @@
       </c>
       <c r="T7" s="17">
         <f t="shared" si="4"/>
-        <v>24.237220491278556</v>
+        <v>24.084197545871582</v>
       </c>
       <c r="W7" s="55">
         <f t="shared" si="5"/>
@@ -4275,9 +4285,9 @@
         <f t="shared" si="11"/>
         <v>3</v>
       </c>
-      <c r="AD7" s="56" t="str">
+      <c r="AD7" s="56">
         <f t="shared" si="12"/>
-        <v/>
+        <v>12</v>
       </c>
       <c r="AE7" s="56" t="str">
         <f t="shared" si="13"/>
@@ -4301,7 +4311,7 @@
       </c>
       <c r="AJ7" s="43">
         <f t="shared" si="18"/>
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4332,7 +4342,9 @@
       <c r="I8" s="35">
         <v>105.3</v>
       </c>
-      <c r="J8" s="36"/>
+      <c r="J8" s="36">
+        <v>118.2</v>
+      </c>
       <c r="K8" s="36"/>
       <c r="L8" s="34"/>
       <c r="M8" s="34"/>
@@ -4340,11 +4352,11 @@
       <c r="O8" s="9"/>
       <c r="P8" s="14">
         <f t="shared" si="0"/>
-        <v>687.09999999999991</v>
+        <v>805.3</v>
       </c>
       <c r="Q8" s="14">
         <f t="shared" si="1"/>
-        <v>98.157142857142844</v>
+        <v>100.66249999999999</v>
       </c>
       <c r="R8" s="15">
         <f t="shared" si="2"/>
@@ -4356,7 +4368,7 @@
       </c>
       <c r="T8" s="15">
         <f t="shared" si="4"/>
-        <v>23.779743280283604</v>
+        <v>23.12808666658664</v>
       </c>
       <c r="W8" s="55">
         <f t="shared" si="5"/>
@@ -4386,9 +4398,9 @@
         <f t="shared" si="11"/>
         <v>8</v>
       </c>
-      <c r="AD8" s="56" t="str">
+      <c r="AD8" s="56">
         <f t="shared" si="12"/>
-        <v/>
+        <v>13</v>
       </c>
       <c r="AE8" s="56" t="str">
         <f t="shared" si="13"/>
@@ -4412,7 +4424,7 @@
       </c>
       <c r="AJ8" s="43">
         <f t="shared" si="18"/>
-        <v>56</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4443,7 +4455,9 @@
       <c r="I9" s="36">
         <v>137.9</v>
       </c>
-      <c r="J9" s="36"/>
+      <c r="J9" s="36">
+        <v>93.4</v>
+      </c>
       <c r="K9" s="36"/>
       <c r="L9" s="36"/>
       <c r="M9" s="36"/>
@@ -4451,11 +4465,11 @@
       <c r="O9" s="8"/>
       <c r="P9" s="16">
         <f t="shared" si="0"/>
-        <v>782.30000000000007</v>
+        <v>875.7</v>
       </c>
       <c r="Q9" s="16">
         <f t="shared" si="1"/>
-        <v>111.75714285714287</v>
+        <v>109.46250000000001</v>
       </c>
       <c r="R9" s="17">
         <f t="shared" si="2"/>
@@ -4467,7 +4481,7 @@
       </c>
       <c r="T9" s="17">
         <f t="shared" si="4"/>
-        <v>29.520267452653389</v>
+        <v>28.090513777531967</v>
       </c>
       <c r="W9" s="55">
         <f t="shared" si="5"/>
@@ -4497,9 +4511,9 @@
         <f t="shared" si="11"/>
         <v>14</v>
       </c>
-      <c r="AD9" s="56" t="str">
+      <c r="AD9" s="56">
         <f t="shared" si="12"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="AE9" s="56" t="str">
         <f t="shared" si="13"/>
@@ -4523,7 +4537,7 @@
       </c>
       <c r="AJ9" s="43">
         <f t="shared" si="18"/>
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4554,7 +4568,9 @@
       <c r="I10" s="34">
         <v>111.4</v>
       </c>
-      <c r="J10" s="34"/>
+      <c r="J10" s="34">
+        <v>94.3</v>
+      </c>
       <c r="K10" s="34"/>
       <c r="L10" s="34"/>
       <c r="M10" s="34"/>
@@ -4562,11 +4578,11 @@
       <c r="O10" s="9"/>
       <c r="P10" s="14">
         <f t="shared" si="0"/>
-        <v>734</v>
+        <v>828.3</v>
       </c>
       <c r="Q10" s="14">
         <f t="shared" si="1"/>
-        <v>104.85714285714286</v>
+        <v>103.53749999999999</v>
       </c>
       <c r="R10" s="15">
         <f t="shared" si="2"/>
@@ -4578,7 +4594,7 @@
       </c>
       <c r="T10" s="15">
         <f t="shared" si="4"/>
-        <v>15.998005828108463</v>
+        <v>15.274342398751235</v>
       </c>
       <c r="W10" s="55">
         <f t="shared" si="5"/>
@@ -4608,9 +4624,9 @@
         <f t="shared" si="11"/>
         <v>9</v>
       </c>
-      <c r="AD10" s="56" t="str">
+      <c r="AD10" s="56">
         <f t="shared" si="12"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="AE10" s="56" t="str">
         <f t="shared" si="13"/>
@@ -4634,7 +4650,7 @@
       </c>
       <c r="AJ10" s="43">
         <f t="shared" si="18"/>
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4665,7 +4681,9 @@
       <c r="I11" s="36">
         <v>124</v>
       </c>
-      <c r="J11" s="36"/>
+      <c r="J11" s="36">
+        <v>99</v>
+      </c>
       <c r="K11" s="36"/>
       <c r="L11" s="36"/>
       <c r="M11" s="36"/>
@@ -4673,11 +4691,11 @@
       <c r="O11" s="8"/>
       <c r="P11" s="16">
         <f t="shared" si="0"/>
-        <v>721.3</v>
+        <v>820.3</v>
       </c>
       <c r="Q11" s="16">
         <f t="shared" si="1"/>
-        <v>103.04285714285713</v>
+        <v>102.53749999999999</v>
       </c>
       <c r="R11" s="17">
         <f t="shared" si="2"/>
@@ -4689,7 +4707,7 @@
       </c>
       <c r="T11" s="17">
         <f t="shared" si="4"/>
-        <v>31.484538911602172</v>
+        <v>29.18404346311771</v>
       </c>
       <c r="W11" s="55">
         <f t="shared" si="5"/>
@@ -4719,9 +4737,9 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="AD11" s="56" t="str">
+      <c r="AD11" s="56">
         <f t="shared" si="12"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="AE11" s="56" t="str">
         <f t="shared" si="13"/>
@@ -4745,7 +4763,7 @@
       </c>
       <c r="AJ11" s="43">
         <f t="shared" si="18"/>
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4776,7 +4794,9 @@
       <c r="I12" s="34">
         <v>69.099999999999994</v>
       </c>
-      <c r="J12" s="34"/>
+      <c r="J12" s="34">
+        <v>92.8</v>
+      </c>
       <c r="K12" s="34"/>
       <c r="L12" s="34"/>
       <c r="M12" s="34"/>
@@ -4784,11 +4804,11 @@
       <c r="O12" s="9"/>
       <c r="P12" s="14">
         <f t="shared" ref="P12:P17" si="19">SUM(C12:O12)</f>
-        <v>730.2</v>
+        <v>823</v>
       </c>
       <c r="Q12" s="14">
         <f t="shared" ref="Q12:Q17" si="20">AVERAGE(C12:O12)</f>
-        <v>104.31428571428572</v>
+        <v>102.875</v>
       </c>
       <c r="R12" s="15">
         <f t="shared" ref="R12:R17" si="21">MAX(C12:O12)</f>
@@ -4800,7 +4820,7 @@
       </c>
       <c r="T12" s="15">
         <f t="shared" ref="T12:T17" si="23">STDEV(C12:O12)</f>
-        <v>24.421945634437648</v>
+        <v>22.973882686961861</v>
       </c>
       <c r="W12" s="55">
         <f t="shared" si="5"/>
@@ -4830,9 +4850,9 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="AD12" s="56" t="str">
+      <c r="AD12" s="56">
         <f t="shared" si="12"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="AE12" s="56" t="str">
         <f t="shared" si="13"/>
@@ -4856,7 +4876,7 @@
       </c>
       <c r="AJ12" s="43">
         <f t="shared" si="18"/>
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4887,7 +4907,9 @@
       <c r="I13" s="36">
         <v>79.7</v>
       </c>
-      <c r="J13" s="36"/>
+      <c r="J13" s="36">
+        <v>97.7</v>
+      </c>
       <c r="K13" s="36"/>
       <c r="L13" s="36"/>
       <c r="M13" s="36"/>
@@ -4895,11 +4917,11 @@
       <c r="O13" s="8"/>
       <c r="P13" s="16">
         <f t="shared" si="19"/>
-        <v>707.90000000000009</v>
+        <v>805.60000000000014</v>
       </c>
       <c r="Q13" s="16">
         <f t="shared" si="20"/>
-        <v>101.12857142857145</v>
+        <v>100.70000000000002</v>
       </c>
       <c r="R13" s="17">
         <f t="shared" si="21"/>
@@ -4911,7 +4933,7 @@
       </c>
       <c r="T13" s="17">
         <f t="shared" si="23"/>
-        <v>18.926939732007497</v>
+        <v>17.564818733560884</v>
       </c>
       <c r="W13" s="55">
         <f t="shared" si="5"/>
@@ -4941,9 +4963,9 @@
         <f t="shared" si="11"/>
         <v>5</v>
       </c>
-      <c r="AD13" s="56" t="str">
+      <c r="AD13" s="56">
         <f t="shared" si="12"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="AE13" s="56" t="str">
         <f t="shared" si="13"/>
@@ -4967,7 +4989,7 @@
       </c>
       <c r="AJ13" s="43">
         <f t="shared" si="18"/>
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4998,7 +5020,9 @@
       <c r="I14" s="34">
         <v>126.5</v>
       </c>
-      <c r="J14" s="34"/>
+      <c r="J14" s="34">
+        <v>115.5</v>
+      </c>
       <c r="K14" s="34"/>
       <c r="L14" s="34"/>
       <c r="M14" s="34"/>
@@ -5006,11 +5030,11 @@
       <c r="O14" s="9"/>
       <c r="P14" s="14">
         <f t="shared" si="19"/>
-        <v>715.3</v>
+        <v>830.8</v>
       </c>
       <c r="Q14" s="14">
         <f t="shared" si="20"/>
-        <v>102.18571428571428</v>
+        <v>103.85</v>
       </c>
       <c r="R14" s="15">
         <f t="shared" si="21"/>
@@ -5022,7 +5046,7 @@
       </c>
       <c r="T14" s="15">
         <f t="shared" si="23"/>
-        <v>15.967616036990801</v>
+        <v>15.514509338035905</v>
       </c>
       <c r="W14" s="55">
         <f t="shared" si="5"/>
@@ -5052,9 +5076,9 @@
         <f t="shared" si="11"/>
         <v>13</v>
       </c>
-      <c r="AD14" s="56" t="str">
+      <c r="AD14" s="56">
         <f t="shared" si="12"/>
-        <v/>
+        <v>11</v>
       </c>
       <c r="AE14" s="56" t="str">
         <f t="shared" si="13"/>
@@ -5078,7 +5102,7 @@
       </c>
       <c r="AJ14" s="43">
         <f t="shared" si="18"/>
-        <v>54</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5109,7 +5133,9 @@
       <c r="I15" s="36">
         <v>115.1</v>
       </c>
-      <c r="J15" s="36"/>
+      <c r="J15" s="36">
+        <v>82.7</v>
+      </c>
       <c r="K15" s="36"/>
       <c r="L15" s="36"/>
       <c r="M15" s="36"/>
@@ -5117,11 +5143,11 @@
       <c r="O15" s="8"/>
       <c r="P15" s="16">
         <f t="shared" si="19"/>
-        <v>687.50000000000011</v>
+        <v>770.20000000000016</v>
       </c>
       <c r="Q15" s="16">
         <f t="shared" si="20"/>
-        <v>98.214285714285737</v>
+        <v>96.27500000000002</v>
       </c>
       <c r="R15" s="17">
         <f t="shared" si="21"/>
@@ -5133,7 +5159,7 @@
       </c>
       <c r="T15" s="17">
         <f t="shared" si="23"/>
-        <v>13.336469869175408</v>
+        <v>13.510710037384444</v>
       </c>
       <c r="W15" s="55">
         <f t="shared" si="5"/>
@@ -5163,9 +5189,9 @@
         <f t="shared" si="11"/>
         <v>10</v>
       </c>
-      <c r="AD15" s="56" t="str">
+      <c r="AD15" s="56">
         <f t="shared" si="12"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="AE15" s="56" t="str">
         <f t="shared" si="13"/>
@@ -5189,7 +5215,7 @@
       </c>
       <c r="AJ15" s="43">
         <f t="shared" si="18"/>
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5220,7 +5246,9 @@
       <c r="I16" s="34">
         <v>120.4</v>
       </c>
-      <c r="J16" s="34"/>
+      <c r="J16" s="34">
+        <v>107.2</v>
+      </c>
       <c r="K16" s="34"/>
       <c r="L16" s="34"/>
       <c r="M16" s="34"/>
@@ -5228,11 +5256,11 @@
       <c r="O16" s="9"/>
       <c r="P16" s="14">
         <f t="shared" si="19"/>
-        <v>672.09999999999991</v>
+        <v>779.3</v>
       </c>
       <c r="Q16" s="14">
         <f t="shared" si="20"/>
-        <v>96.014285714285705</v>
+        <v>97.412499999999994</v>
       </c>
       <c r="R16" s="15">
         <f t="shared" si="21"/>
@@ -5244,7 +5272,7 @@
       </c>
       <c r="T16" s="15">
         <f t="shared" si="23"/>
-        <v>20.662883678343789</v>
+        <v>19.534616709830853</v>
       </c>
       <c r="W16" s="55">
         <f t="shared" si="5"/>
@@ -5274,9 +5302,9 @@
         <f t="shared" si="11"/>
         <v>11</v>
       </c>
-      <c r="AD16" s="56" t="str">
+      <c r="AD16" s="56">
         <f t="shared" si="12"/>
-        <v/>
+        <v>10</v>
       </c>
       <c r="AE16" s="56" t="str">
         <f t="shared" si="13"/>
@@ -5300,7 +5328,7 @@
       </c>
       <c r="AJ16" s="43">
         <f t="shared" si="18"/>
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:41" ht="24" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5496,11 +5524,11 @@
     <row r="19" spans="1:41" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P19" s="11">
         <f>SUM(C3:O18)</f>
-        <v>9745.6000000000022</v>
+        <v>11165.100000000002</v>
       </c>
       <c r="Q19" s="11">
         <f>AVERAGE(C3:O18)</f>
-        <v>99.444897959183692</v>
+        <v>99.688392857142873</v>
       </c>
       <c r="R19" s="18">
         <f>MAX(C3:O18)</f>
@@ -5512,7 +5540,7 @@
       </c>
       <c r="T19" s="18">
         <f>STDEV(C3:O18)</f>
-        <v>21.871372441246123</v>
+        <v>20.920694291683386</v>
       </c>
     </row>
     <row r="20" spans="1:41" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -5567,23 +5595,21 @@
         <v>Spos Before Hos</v>
       </c>
       <c r="C22" s="21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D22" s="46">
         <f>AJ3</f>
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E22" s="49">
         <f t="shared" ref="E22:E31" si="24">IF(D3="",-99,IF(T3=0,1,(Q3-$Q$19)/T3))</f>
-        <v>1.3167574075723558</v>
+        <v>0.96371290422986977</v>
       </c>
       <c r="F22" s="28">
         <f>IF(C3="",0,Q3)</f>
-        <v>116.2</v>
-      </c>
-      <c r="G22" s="39">
-        <v>100</v>
-      </c>
+        <v>113.3875</v>
+      </c>
+      <c r="G22" s="39"/>
       <c r="H22" s="22">
         <f>IF(C22="",16,RANK(C22,$C$22:$C$37,0))</f>
         <v>1</v>
@@ -5602,7 +5628,7 @@
       </c>
       <c r="L22" s="22">
         <f t="shared" ref="L22" si="25">IF(G22="",16,RANK(G22,$G$22:$G$37,0))</f>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="N22" s="104"/>
       <c r="O22" s="104"/>
@@ -5624,22 +5650,20 @@
       </c>
       <c r="D23" s="47">
         <f t="shared" ref="D23:D37" si="26">AJ4</f>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E23" s="50">
         <f t="shared" si="24"/>
-        <v>-0.38665806098968752</v>
+        <v>-0.46226938458763051</v>
       </c>
       <c r="F23" s="28">
         <f t="shared" ref="F23:F37" si="27">IF(C4="",0,Q4)</f>
-        <v>89</v>
-      </c>
-      <c r="G23" s="40">
-        <v>78</v>
-      </c>
+        <v>88.0625</v>
+      </c>
+      <c r="G23" s="40"/>
       <c r="H23" s="24">
         <f t="shared" ref="H23:H37" si="28">IF(C23="",16,RANK(C23,$C$22:$C$37,0))</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I23" s="24">
         <f t="shared" ref="I23:I37" si="29">IF(C23="",16,RANK(D23,$D$22:$D$37,0))</f>
@@ -5655,7 +5679,7 @@
       </c>
       <c r="L23" s="24">
         <f t="shared" ref="L23:L37" si="31">IF(G23="",16,RANK(G23,$G$22:$G$37,0))</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="N23" s="30"/>
       <c r="O23" s="30"/>
@@ -5669,30 +5693,28 @@
         <v>SUPERMAX LOCO</v>
       </c>
       <c r="C24" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" s="47">
         <f t="shared" si="26"/>
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E24" s="50">
         <f t="shared" si="24"/>
-        <v>-1.2844137559218278</v>
+        <v>-0.9681214417243319</v>
       </c>
       <c r="F24" s="28">
         <f t="shared" si="27"/>
-        <v>79.914285714285725</v>
-      </c>
-      <c r="G24" s="40">
-        <v>81.599999999999994</v>
-      </c>
+        <v>83.262500000000017</v>
+      </c>
+      <c r="G24" s="40"/>
       <c r="H24" s="24">
         <f t="shared" si="28"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I24" s="24">
         <f t="shared" si="29"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J24" s="24">
         <f>RANK(E24,$E$22:$E39,0)</f>
@@ -5704,7 +5726,7 @@
       </c>
       <c r="L24" s="24">
         <f t="shared" si="31"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N24" s="104" t="s">
         <v>44</v>
@@ -5730,42 +5752,40 @@
         <v>Team Thomas</v>
       </c>
       <c r="C25" s="23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D25" s="47">
         <f t="shared" si="26"/>
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="E25" s="50">
         <f t="shared" si="24"/>
-        <v>-0.29947560459739103</v>
+        <v>-0.11669415265817819</v>
       </c>
       <c r="F25" s="28">
         <f t="shared" si="27"/>
-        <v>94.585714285714289</v>
-      </c>
-      <c r="G25" s="40">
-        <v>94.4</v>
-      </c>
+        <v>97.662500000000009</v>
+      </c>
+      <c r="G25" s="40"/>
       <c r="H25" s="24">
         <f t="shared" si="28"/>
         <v>7</v>
       </c>
       <c r="I25" s="24">
         <f t="shared" si="29"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J25" s="24">
         <f>RANK(E25,$E$22:$E40,0)</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K25" s="24">
         <f t="shared" si="30"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L25" s="24">
         <f t="shared" si="31"/>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="N25" s="104"/>
       <c r="O25" s="104"/>
@@ -5793,26 +5813,24 @@
       </c>
       <c r="D26" s="47">
         <f t="shared" si="26"/>
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="E26" s="50">
         <f t="shared" si="24"/>
-        <v>-0.27180324181196158</v>
+        <v>-0.15522181505207244</v>
       </c>
       <c r="F26" s="28">
         <f t="shared" si="27"/>
-        <v>92.857142857142875</v>
-      </c>
-      <c r="G26" s="40">
-        <v>92.6</v>
-      </c>
+        <v>95.950000000000017</v>
+      </c>
+      <c r="G26" s="40"/>
       <c r="H26" s="24">
         <f t="shared" si="28"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I26" s="24">
         <f t="shared" si="29"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J26" s="24">
         <f>RANK(E26,$E$22:$E41,0)</f>
@@ -5824,7 +5842,7 @@
       </c>
       <c r="L26" s="24">
         <f t="shared" si="31"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="N26" s="30"/>
       <c r="O26" s="30"/>
@@ -5838,30 +5856,28 @@
         <v>Deflate Deez Nutz</v>
       </c>
       <c r="C27" s="23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D27" s="47">
         <f t="shared" si="26"/>
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="E27" s="50">
         <f t="shared" si="24"/>
-        <v>-5.4153448456634869E-2</v>
+        <v>4.2117930328600131E-2</v>
       </c>
       <c r="F27" s="28">
         <f t="shared" si="27"/>
-        <v>98.157142857142844</v>
-      </c>
-      <c r="G27" s="40">
-        <v>89</v>
-      </c>
+        <v>100.66249999999999</v>
+      </c>
+      <c r="G27" s="40"/>
       <c r="H27" s="24">
         <f t="shared" si="28"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I27" s="24">
         <f t="shared" si="29"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J27" s="24">
         <f>RANK(E27,$E$22:$E42,0)</f>
@@ -5869,11 +5885,11 @@
       </c>
       <c r="K27" s="24">
         <f t="shared" si="30"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L27" s="24">
         <f t="shared" si="31"/>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="N27" s="100" t="s">
         <v>45</v>
@@ -5897,26 +5913,24 @@
       </c>
       <c r="D28" s="47">
         <f t="shared" si="26"/>
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E28" s="50">
         <f t="shared" si="24"/>
-        <v>0.41707768798864681</v>
+        <v>0.34795045830293414</v>
       </c>
       <c r="F28" s="28">
         <f t="shared" si="27"/>
-        <v>111.75714285714287</v>
-      </c>
-      <c r="G28" s="40">
-        <v>87.6</v>
-      </c>
+        <v>109.46250000000001</v>
+      </c>
+      <c r="G28" s="40"/>
       <c r="H28" s="24">
         <f t="shared" si="28"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I28" s="24">
         <f t="shared" si="29"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J28" s="24">
         <f>RANK(E28,$E$22:$E43,0)</f>
@@ -5928,7 +5942,7 @@
       </c>
       <c r="L28" s="24">
         <f t="shared" si="31"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="N28" s="100"/>
       <c r="O28" s="100"/>
@@ -5946,42 +5960,37 @@
         <v>Team Wasserman</v>
       </c>
       <c r="C29" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" s="47">
         <f t="shared" si="26"/>
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E29" s="50">
         <f t="shared" si="24"/>
-        <v>0.33830747132557398</v>
+        <v>0.25199822305749858</v>
       </c>
       <c r="F29" s="28">
         <f t="shared" si="27"/>
-        <v>104.85714285714286</v>
-      </c>
-      <c r="G29" s="40">
-        <v>95.3</v>
-      </c>
+        <v>103.53749999999999</v>
+      </c>
+      <c r="G29" s="40"/>
       <c r="H29" s="24">
         <f t="shared" si="28"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I29" s="24">
         <f t="shared" si="29"/>
         <v>4</v>
       </c>
-      <c r="J29" s="24">
-        <f>RANK(E29,$E$22:$E44,0)</f>
-        <v>3</v>
-      </c>
+      <c r="J29" s="24"/>
       <c r="K29" s="24">
         <f t="shared" si="30"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L29" s="24">
         <f t="shared" si="31"/>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="N29" s="100"/>
       <c r="O29" s="100"/>
@@ -6003,26 +6012,24 @@
       </c>
       <c r="D30" s="47">
         <f t="shared" si="26"/>
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E30" s="50">
         <f t="shared" si="24"/>
-        <v>0.11427701684865955</v>
+        <v>9.762551054509544E-2</v>
       </c>
       <c r="F30" s="28">
         <f t="shared" si="27"/>
-        <v>103.04285714285713</v>
-      </c>
-      <c r="G30" s="40">
-        <v>93.9</v>
-      </c>
+        <v>102.53749999999999</v>
+      </c>
+      <c r="G30" s="40"/>
       <c r="H30" s="24">
         <f t="shared" si="28"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I30" s="24">
         <f t="shared" si="29"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J30" s="24">
         <f>RANK(E30,$E$22:$E45,0)</f>
@@ -6030,11 +6037,11 @@
       </c>
       <c r="K30" s="24">
         <f t="shared" si="30"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L30" s="24">
         <f t="shared" si="31"/>
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="N30" s="100"/>
       <c r="O30" s="100"/>
@@ -6056,38 +6063,36 @@
       </c>
       <c r="D31" s="47">
         <f t="shared" si="26"/>
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E31" s="50">
         <f t="shared" si="24"/>
-        <v>0.19938574215133986</v>
+        <v>0.13870564180540501</v>
       </c>
       <c r="F31" s="28">
         <f t="shared" si="27"/>
-        <v>104.31428571428572</v>
-      </c>
-      <c r="G31" s="40">
-        <v>95.1</v>
-      </c>
+        <v>102.875</v>
+      </c>
+      <c r="G31" s="40"/>
       <c r="H31" s="24">
         <f t="shared" si="28"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I31" s="24">
         <f t="shared" si="29"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J31" s="24">
         <f>RANK(E31,$E$22:$E46,0)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K31" s="24">
         <f t="shared" si="30"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L31" s="24">
         <f t="shared" si="31"/>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="N31" s="100"/>
       <c r="O31" s="100"/>
@@ -6109,22 +6114,20 @@
       </c>
       <c r="D32" s="47">
         <f t="shared" si="26"/>
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E32" s="50">
         <f>IF(D13="",-99,IF(T13=0,1,(Q13-$Q$19)/T13))</f>
-        <v>8.8956455360846454E-2</v>
+        <v>5.7592802875003721E-2</v>
       </c>
       <c r="F32" s="28">
         <f t="shared" si="27"/>
-        <v>101.12857142857145</v>
-      </c>
-      <c r="G32" s="40">
-        <v>85.2</v>
-      </c>
+        <v>100.70000000000002</v>
+      </c>
+      <c r="G32" s="40"/>
       <c r="H32" s="24">
         <f t="shared" si="28"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I32" s="24">
         <f t="shared" si="29"/>
@@ -6140,7 +6143,7 @@
       </c>
       <c r="L32" s="24">
         <f t="shared" si="31"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="N32" s="77"/>
       <c r="O32" s="77"/>
@@ -6158,42 +6161,40 @@
         <v>Cool Hand Lou</v>
       </c>
       <c r="C33" s="23">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D33" s="47">
         <f t="shared" si="26"/>
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="E33" s="50">
         <f t="shared" ref="E33:E37" si="32">IF(D14="",-99,IF(T14=0,1,(Q14-$Q$19)/T14))</f>
-        <v>0.17164843644669175</v>
+        <v>0.26823968790649294</v>
       </c>
       <c r="F33" s="28">
         <f t="shared" si="27"/>
-        <v>102.18571428571428</v>
-      </c>
-      <c r="G33" s="40">
-        <v>96.4</v>
-      </c>
+        <v>103.85</v>
+      </c>
+      <c r="G33" s="40"/>
       <c r="H33" s="24">
         <f t="shared" si="28"/>
         <v>2</v>
       </c>
       <c r="I33" s="24">
         <f t="shared" si="29"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J33" s="24">
         <f>RANK(E33,$E$22:$E48,0)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K33" s="24">
         <f t="shared" si="30"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L33" s="24">
         <f t="shared" si="31"/>
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="N33" s="100" t="s">
         <v>47</v>
@@ -6217,38 +6218,36 @@
       </c>
       <c r="D34" s="47">
         <f t="shared" si="26"/>
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E34" s="50">
         <f t="shared" si="32"/>
-        <v>-9.2274211764409253E-2</v>
+        <v>-0.25264348414686694</v>
       </c>
       <c r="F34" s="28">
         <f t="shared" si="27"/>
-        <v>98.214285714285737</v>
-      </c>
-      <c r="G34" s="40">
-        <v>99</v>
-      </c>
+        <v>96.27500000000002</v>
+      </c>
+      <c r="G34" s="40"/>
       <c r="H34" s="24">
         <f t="shared" si="28"/>
         <v>12</v>
       </c>
       <c r="I34" s="24">
         <f t="shared" si="29"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J34" s="24">
         <f>RANK(E34,$E$22:$E49,0)</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="K34" s="24">
         <f t="shared" si="30"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="L34" s="24">
         <f t="shared" si="31"/>
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="N34" s="100"/>
       <c r="O34" s="100"/>
@@ -6266,23 +6265,21 @@
         <v>Team Force</v>
       </c>
       <c r="C35" s="23">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D35" s="47">
         <f t="shared" si="26"/>
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="E35" s="50">
         <f t="shared" si="32"/>
-        <v>-0.16602775770806466</v>
+        <v>-0.11650563156417236</v>
       </c>
       <c r="F35" s="28">
         <f t="shared" si="27"/>
-        <v>96.014285714285705</v>
-      </c>
-      <c r="G35" s="40">
-        <v>89.8</v>
-      </c>
+        <v>97.412499999999994</v>
+      </c>
+      <c r="G35" s="40"/>
       <c r="H35" s="24">
         <f t="shared" si="28"/>
         <v>2</v>
@@ -6293,7 +6290,7 @@
       </c>
       <c r="J35" s="24">
         <f>RANK(E35,$E$22:$E50,0)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K35" s="24">
         <f t="shared" si="30"/>
@@ -6301,7 +6298,7 @@
       </c>
       <c r="L35" s="24">
         <f t="shared" si="31"/>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="N35" s="100"/>
       <c r="O35" s="100"/>
@@ -6562,7 +6559,7 @@
       </c>
       <c r="D3" s="82">
         <f t="shared" ref="D3:D18" si="1">AVERAGE(3*E3,F3,G3,H3,I3)</f>
-        <v>1.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E3" s="83">
         <f>POINTS!H22</f>
@@ -6582,7 +6579,7 @@
       </c>
       <c r="I3" s="84">
         <f>POINTS!L22</f>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="J3" s="78"/>
     </row>
@@ -6593,15 +6590,15 @@
       </c>
       <c r="C4" s="71">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="85">
         <f t="shared" si="1"/>
-        <v>14.8</v>
+        <v>15.8</v>
       </c>
       <c r="E4" s="86">
         <f>POINTS!H23</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F4" s="86">
         <f>POINTS!I23</f>
@@ -6617,7 +6614,7 @@
       </c>
       <c r="I4" s="87">
         <f>POINTS!L23</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J4" s="79"/>
     </row>
@@ -6632,15 +6629,15 @@
       </c>
       <c r="D5" s="85">
         <f t="shared" si="1"/>
-        <v>18.8</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="E5" s="86">
         <f>POINTS!H24</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="86">
         <f>POINTS!I24</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="86">
         <f>POINTS!J24</f>
@@ -6652,7 +6649,7 @@
       </c>
       <c r="I5" s="87">
         <f>POINTS!L24</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J5" s="79"/>
     </row>
@@ -6667,7 +6664,7 @@
       </c>
       <c r="D6" s="85">
         <f t="shared" si="1"/>
-        <v>12.2</v>
+        <v>13</v>
       </c>
       <c r="E6" s="86">
         <f>POINTS!H25</f>
@@ -6675,19 +6672,19 @@
       </c>
       <c r="F6" s="86">
         <f>POINTS!I25</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G6" s="86">
         <f>POINTS!J25</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H6" s="86">
         <f>POINTS!K25</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I6" s="87">
         <f>POINTS!L25</f>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="J6" s="79"/>
     </row>
@@ -6702,15 +6699,15 @@
       </c>
       <c r="D7" s="85">
         <f t="shared" si="1"/>
-        <v>12.8</v>
+        <v>14.8</v>
       </c>
       <c r="E7" s="86">
         <f>POINTS!H26</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F7" s="86">
         <f>POINTS!I26</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="86">
         <f>POINTS!J26</f>
@@ -6722,7 +6719,7 @@
       </c>
       <c r="I7" s="87">
         <f>POINTS!L26</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J7" s="79"/>
     </row>
@@ -6733,19 +6730,19 @@
       </c>
       <c r="C8" s="71">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D8" s="85">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E8" s="86">
         <f>POINTS!H27</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F8" s="86">
         <f>POINTS!I27</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G8" s="86">
         <f>POINTS!J27</f>
@@ -6753,11 +6750,11 @@
       </c>
       <c r="H8" s="86">
         <f>POINTS!K27</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I8" s="87">
         <f>POINTS!L27</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J8" s="79"/>
     </row>
@@ -6768,19 +6765,19 @@
       </c>
       <c r="C9" s="71">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9" s="85">
         <f t="shared" si="1"/>
-        <v>4.5999999999999996</v>
+        <v>7</v>
       </c>
       <c r="E9" s="86">
         <f>POINTS!H28</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F9" s="86">
         <f>POINTS!I28</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G9" s="86">
         <f>POINTS!J28</f>
@@ -6792,7 +6789,7 @@
       </c>
       <c r="I9" s="87">
         <f>POINTS!L28</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J9" s="79"/>
     </row>
@@ -6807,11 +6804,11 @@
       </c>
       <c r="D10" s="85">
         <f t="shared" si="1"/>
-        <v>10.6</v>
+        <v>12</v>
       </c>
       <c r="E10" s="86">
         <f>POINTS!H29</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10" s="86">
         <f>POINTS!I29</f>
@@ -6819,15 +6816,15 @@
       </c>
       <c r="G10" s="86">
         <f>POINTS!J29</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H10" s="86">
         <f>POINTS!K29</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I10" s="87">
         <f>POINTS!L29</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J10" s="79"/>
     </row>
@@ -6838,19 +6835,19 @@
       </c>
       <c r="C11" s="71">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D11" s="85">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>11.8</v>
       </c>
       <c r="E11" s="86">
         <f>POINTS!H30</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F11" s="86">
         <f>POINTS!I30</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G11" s="86">
         <f>POINTS!J30</f>
@@ -6858,11 +6855,11 @@
       </c>
       <c r="H11" s="86">
         <f>POINTS!K30</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I11" s="87">
         <f>POINTS!L30</f>
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="J11" s="79"/>
     </row>
@@ -6873,31 +6870,31 @@
       </c>
       <c r="C12" s="71">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D12" s="85">
         <f t="shared" si="1"/>
-        <v>7.4</v>
+        <v>11</v>
       </c>
       <c r="E12" s="86">
         <f>POINTS!H31</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F12" s="86">
         <f>POINTS!I31</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G12" s="86">
         <f>POINTS!J31</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H12" s="86">
         <f>POINTS!K31</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I12" s="87">
         <f>POINTS!L31</f>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="J12" s="79"/>
     </row>
@@ -6912,11 +6909,11 @@
       </c>
       <c r="D13" s="85">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E13" s="86">
         <f>POINTS!H32</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F13" s="86">
         <f>POINTS!I32</f>
@@ -6932,7 +6929,7 @@
       </c>
       <c r="I13" s="87">
         <f>POINTS!L32</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J13" s="79"/>
     </row>
@@ -6943,11 +6940,11 @@
       </c>
       <c r="C14" s="71">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="85">
         <f t="shared" si="1"/>
-        <v>5.2</v>
+        <v>6.6</v>
       </c>
       <c r="E14" s="86">
         <f>POINTS!H33</f>
@@ -6955,19 +6952,19 @@
       </c>
       <c r="F14" s="86">
         <f>POINTS!I33</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G14" s="86">
         <f>POINTS!J33</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H14" s="86">
         <f>POINTS!K33</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I14" s="87">
         <f>POINTS!L33</f>
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="J14" s="79"/>
     </row>
@@ -6978,11 +6975,11 @@
       </c>
       <c r="C15" s="71">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D15" s="85">
         <f t="shared" si="1"/>
-        <v>12.8</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="E15" s="86">
         <f>POINTS!H34</f>
@@ -6990,19 +6987,19 @@
       </c>
       <c r="F15" s="86">
         <f>POINTS!I34</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G15" s="86">
         <f>POINTS!J34</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H15" s="86">
         <f>POINTS!K34</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I15" s="87">
         <f>POINTS!L34</f>
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="J15" s="79"/>
     </row>
@@ -7017,7 +7014,7 @@
       </c>
       <c r="D16" s="85">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="E16" s="86">
         <f>POINTS!H35</f>
@@ -7029,7 +7026,7 @@
       </c>
       <c r="G16" s="86">
         <f>POINTS!J35</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H16" s="86">
         <f>POINTS!K35</f>
@@ -7037,7 +7034,7 @@
       </c>
       <c r="I16" s="87">
         <f>POINTS!L35</f>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="J16" s="79"/>
     </row>
@@ -7129,7 +7126,7 @@
   <dimension ref="B2:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I16"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -7182,7 +7179,7 @@
       </c>
       <c r="D3" s="82">
         <f>AVERAGE(3*E3,F3,G3,H3,I3)</f>
-        <v>1.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E3" s="83">
         <f>POINTS!H22</f>
@@ -7202,14 +7199,14 @@
       </c>
       <c r="I3" s="84">
         <f>POINTS!L22</f>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="J3" s="78"/>
     </row>
     <row r="4" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B4" s="92" t="str">
-        <f>POINTS!B9</f>
-        <v>Team Gregory</v>
+        <f>POINTS!B14</f>
+        <v>Cool Hand Lou</v>
       </c>
       <c r="C4" s="71">
         <f>RANK(D4,$D$3:$D$16,1)</f>
@@ -7217,34 +7214,34 @@
       </c>
       <c r="D4" s="85">
         <f>AVERAGE(3*E4,F4,G4,H4,I4)</f>
-        <v>4.5999999999999996</v>
+        <v>6.6</v>
       </c>
       <c r="E4" s="86">
-        <f>POINTS!H28</f>
+        <f>POINTS!H33</f>
         <v>2</v>
       </c>
       <c r="F4" s="86">
-        <f>POINTS!I28</f>
-        <v>2</v>
+        <f>POINTS!I33</f>
+        <v>5</v>
       </c>
       <c r="G4" s="86">
-        <f>POINTS!J28</f>
-        <v>2</v>
+        <f>POINTS!J33</f>
+        <v>3</v>
       </c>
       <c r="H4" s="86">
-        <f>POINTS!K28</f>
-        <v>2</v>
+        <f>POINTS!K33</f>
+        <v>3</v>
       </c>
       <c r="I4" s="87">
-        <f>POINTS!L28</f>
-        <v>11</v>
+        <f>POINTS!L33</f>
+        <v>16</v>
       </c>
       <c r="J4" s="79"/>
     </row>
     <row r="5" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B5" s="92" t="str">
-        <f>POINTS!B14</f>
-        <v>Cool Hand Lou</v>
+        <f>POINTS!B9</f>
+        <v>Team Gregory</v>
       </c>
       <c r="C5" s="71">
         <f>RANK(D5,$D$3:$D$16,1)</f>
@@ -7252,34 +7249,34 @@
       </c>
       <c r="D5" s="85">
         <f>AVERAGE(3*E5,F5,G5,H5,I5)</f>
-        <v>5.2</v>
+        <v>7</v>
       </c>
       <c r="E5" s="86">
-        <f>POINTS!H33</f>
+        <f>POINTS!H28</f>
+        <v>4</v>
+      </c>
+      <c r="F5" s="86">
+        <f>POINTS!I28</f>
+        <v>3</v>
+      </c>
+      <c r="G5" s="86">
+        <f>POINTS!J28</f>
         <v>2</v>
       </c>
-      <c r="F5" s="86">
-        <f>POINTS!I33</f>
-        <v>6</v>
-      </c>
-      <c r="G5" s="86">
-        <f>POINTS!J33</f>
-        <v>5</v>
-      </c>
       <c r="H5" s="86">
-        <f>POINTS!K33</f>
-        <v>6</v>
+        <f>POINTS!K28</f>
+        <v>2</v>
       </c>
       <c r="I5" s="87">
-        <f>POINTS!L33</f>
-        <v>3</v>
+        <f>POINTS!L28</f>
+        <v>16</v>
       </c>
       <c r="J5" s="79"/>
     </row>
     <row r="6" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B6" s="92" t="str">
-        <f>POINTS!B12</f>
-        <v>Team Frisch</v>
+        <f>POINTS!B8</f>
+        <v>Deflate Deez Nutz</v>
       </c>
       <c r="C6" s="71">
         <f>RANK(D6,$D$3:$D$16,1)</f>
@@ -7287,69 +7284,69 @@
       </c>
       <c r="D6" s="85">
         <f>AVERAGE(3*E6,F6,G6,H6,I6)</f>
-        <v>7.4</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E6" s="86">
-        <f>POINTS!H31</f>
-        <v>7</v>
+        <f>POINTS!H27</f>
+        <v>4</v>
       </c>
       <c r="F6" s="86">
-        <f>POINTS!I31</f>
-        <v>3</v>
+        <f>POINTS!I27</f>
+        <v>2</v>
       </c>
       <c r="G6" s="86">
-        <f>POINTS!J31</f>
-        <v>4</v>
+        <f>POINTS!J27</f>
+        <v>8</v>
       </c>
       <c r="H6" s="86">
-        <f>POINTS!K31</f>
-        <v>4</v>
+        <f>POINTS!K27</f>
+        <v>8</v>
       </c>
       <c r="I6" s="87">
-        <f>POINTS!L31</f>
-        <v>5</v>
+        <f>POINTS!L27</f>
+        <v>16</v>
       </c>
       <c r="J6" s="79"/>
     </row>
     <row r="7" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B7" s="92" t="str">
-        <f>POINTS!B13</f>
-        <v>OhNo Romo</v>
+        <f>POINTS!B12</f>
+        <v>Team Frisch</v>
       </c>
       <c r="C7" s="71">
         <f>RANK(D7,$D$3:$D$16,1)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D7" s="85">
         <f>AVERAGE(3*E7,F7,G7,H7,I7)</f>
+        <v>11</v>
+      </c>
+      <c r="E7" s="86">
+        <f>POINTS!H31</f>
         <v>8</v>
       </c>
-      <c r="E7" s="86">
-        <f>POINTS!H32</f>
-        <v>2</v>
-      </c>
       <c r="F7" s="86">
-        <f>POINTS!I32</f>
-        <v>8</v>
+        <f>POINTS!I31</f>
+        <v>5</v>
       </c>
       <c r="G7" s="86">
-        <f>POINTS!J32</f>
-        <v>7</v>
+        <f>POINTS!J31</f>
+        <v>5</v>
       </c>
       <c r="H7" s="86">
-        <f>POINTS!K32</f>
-        <v>7</v>
+        <f>POINTS!K31</f>
+        <v>5</v>
       </c>
       <c r="I7" s="87">
-        <f>POINTS!L32</f>
-        <v>12</v>
+        <f>POINTS!L31</f>
+        <v>16</v>
       </c>
       <c r="J7" s="79"/>
     </row>
     <row r="8" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B8" s="92" t="str">
-        <f>POINTS!B11</f>
-        <v>SFV Aguilar</v>
+        <f>POINTS!B16</f>
+        <v>Team Force</v>
       </c>
       <c r="C8" s="71">
         <f>RANK(D8,$D$3:$D$16,1)</f>
@@ -7357,132 +7354,132 @@
       </c>
       <c r="D8" s="85">
         <f>AVERAGE(3*E8,F8,G8,H8,I8)</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="E8" s="86">
+        <f>POINTS!H35</f>
+        <v>2</v>
+      </c>
+      <c r="F8" s="86">
+        <f>POINTS!I35</f>
+        <v>10</v>
+      </c>
+      <c r="G8" s="86">
+        <f>POINTS!J35</f>
         <v>9</v>
       </c>
-      <c r="E8" s="86">
+      <c r="H8" s="86">
+        <f>POINTS!K35</f>
+        <v>10</v>
+      </c>
+      <c r="I8" s="87">
+        <f>POINTS!L35</f>
+        <v>16</v>
+      </c>
+      <c r="J8" s="79"/>
+    </row>
+    <row r="9" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B9" s="92" t="str">
+        <f>POINTS!B13</f>
+        <v>OhNo Romo</v>
+      </c>
+      <c r="C9" s="71">
+        <f>RANK(D9,$D$3:$D$16,1)</f>
+        <v>5</v>
+      </c>
+      <c r="D9" s="85">
+        <f>AVERAGE(3*E9,F9,G9,H9,I9)</f>
+        <v>10</v>
+      </c>
+      <c r="E9" s="86">
+        <f>POINTS!H32</f>
+        <v>4</v>
+      </c>
+      <c r="F9" s="86">
+        <f>POINTS!I32</f>
+        <v>8</v>
+      </c>
+      <c r="G9" s="86">
+        <f>POINTS!J32</f>
+        <v>7</v>
+      </c>
+      <c r="H9" s="86">
+        <f>POINTS!K32</f>
+        <v>7</v>
+      </c>
+      <c r="I9" s="87">
+        <f>POINTS!L32</f>
+        <v>16</v>
+      </c>
+      <c r="J9" s="79"/>
+    </row>
+    <row r="10" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B10" s="92" t="str">
+        <f>POINTS!B10</f>
+        <v>Team Wasserman</v>
+      </c>
+      <c r="C10" s="71">
+        <f>RANK(D10,$D$3:$D$16,1)</f>
+        <v>9</v>
+      </c>
+      <c r="D10" s="85">
+        <f>AVERAGE(3*E10,F10,G10,H10,I10)</f>
+        <v>12</v>
+      </c>
+      <c r="E10" s="86">
+        <f>POINTS!H29</f>
+        <v>12</v>
+      </c>
+      <c r="F10" s="86">
+        <f>POINTS!I29</f>
+        <v>4</v>
+      </c>
+      <c r="G10" s="86">
+        <f>POINTS!J29</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="86">
+        <f>POINTS!K29</f>
+        <v>4</v>
+      </c>
+      <c r="I10" s="87">
+        <f>POINTS!L29</f>
+        <v>16</v>
+      </c>
+      <c r="J10" s="79"/>
+    </row>
+    <row r="11" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B11" s="92" t="str">
+        <f>POINTS!B11</f>
+        <v>SFV Aguilar</v>
+      </c>
+      <c r="C11" s="71">
+        <f>RANK(D11,$D$3:$D$16,1)</f>
+        <v>8</v>
+      </c>
+      <c r="D11" s="85">
+        <f>AVERAGE(3*E11,F11,G11,H11,I11)</f>
+        <v>11.8</v>
+      </c>
+      <c r="E11" s="86">
         <f>POINTS!H30</f>
+        <v>8</v>
+      </c>
+      <c r="F11" s="86">
+        <f>POINTS!I30</f>
         <v>7</v>
       </c>
-      <c r="F8" s="86">
-        <f>POINTS!I30</f>
-        <v>6</v>
-      </c>
-      <c r="G8" s="86">
+      <c r="G11" s="86">
         <f>POINTS!J30</f>
         <v>6</v>
       </c>
-      <c r="H8" s="86">
+      <c r="H11" s="86">
         <f>POINTS!K30</f>
-        <v>5</v>
-      </c>
-      <c r="I8" s="87">
+        <v>6</v>
+      </c>
+      <c r="I11" s="87">
         <f>POINTS!L30</f>
-        <v>7</v>
-      </c>
-      <c r="J8" s="79"/>
-    </row>
-    <row r="9" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B9" s="92" t="str">
-        <f>POINTS!B16</f>
-        <v>Team Force</v>
-      </c>
-      <c r="C9" s="71">
-        <f>RANK(D9,$D$3:$D$16,1)</f>
-        <v>6</v>
-      </c>
-      <c r="D9" s="85">
-        <f>AVERAGE(3*E9,F9,G9,H9,I9)</f>
-        <v>9</v>
-      </c>
-      <c r="E9" s="86">
-        <f>POINTS!H35</f>
-        <v>2</v>
-      </c>
-      <c r="F9" s="86">
-        <f>POINTS!I35</f>
-        <v>10</v>
-      </c>
-      <c r="G9" s="86">
-        <f>POINTS!J35</f>
-        <v>10</v>
-      </c>
-      <c r="H9" s="86">
-        <f>POINTS!K35</f>
-        <v>10</v>
-      </c>
-      <c r="I9" s="87">
-        <f>POINTS!L35</f>
-        <v>9</v>
-      </c>
-      <c r="J9" s="79"/>
-    </row>
-    <row r="10" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B10" s="92" t="str">
-        <f>POINTS!B8</f>
-        <v>Deflate Deez Nutz</v>
-      </c>
-      <c r="C10" s="71">
-        <f>RANK(D10,$D$3:$D$16,1)</f>
-        <v>8</v>
-      </c>
-      <c r="D10" s="85">
-        <f>AVERAGE(3*E10,F10,G10,H10,I10)</f>
-        <v>10</v>
-      </c>
-      <c r="E10" s="86">
-        <f>POINTS!H27</f>
-        <v>6</v>
-      </c>
-      <c r="F10" s="86">
-        <f>POINTS!I27</f>
-        <v>5</v>
-      </c>
-      <c r="G10" s="86">
-        <f>POINTS!J27</f>
-        <v>8</v>
-      </c>
-      <c r="H10" s="86">
-        <f>POINTS!K27</f>
-        <v>9</v>
-      </c>
-      <c r="I10" s="87">
-        <f>POINTS!L27</f>
-        <v>10</v>
-      </c>
-      <c r="J10" s="79"/>
-    </row>
-    <row r="11" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B11" s="92" t="str">
-        <f>POINTS!B10</f>
-        <v>Team Wasserman</v>
-      </c>
-      <c r="C11" s="71">
-        <f>RANK(D11,$D$3:$D$16,1)</f>
-        <v>9</v>
-      </c>
-      <c r="D11" s="85">
-        <f>AVERAGE(3*E11,F11,G11,H11,I11)</f>
-        <v>10.6</v>
-      </c>
-      <c r="E11" s="86">
-        <f>POINTS!H29</f>
-        <v>13</v>
-      </c>
-      <c r="F11" s="86">
-        <f>POINTS!I29</f>
-        <v>4</v>
-      </c>
-      <c r="G11" s="86">
-        <f>POINTS!J29</f>
-        <v>3</v>
-      </c>
-      <c r="H11" s="86">
-        <f>POINTS!K29</f>
-        <v>3</v>
-      </c>
-      <c r="I11" s="87">
-        <f>POINTS!L29</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J11" s="79"/>
     </row>
@@ -7497,7 +7494,7 @@
       </c>
       <c r="D12" s="85">
         <f>AVERAGE(3*E12,F12,G12,H12,I12)</f>
-        <v>12.2</v>
+        <v>13</v>
       </c>
       <c r="E12" s="86">
         <f>POINTS!H25</f>
@@ -7505,19 +7502,19 @@
       </c>
       <c r="F12" s="86">
         <f>POINTS!I25</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G12" s="86">
         <f>POINTS!J25</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H12" s="86">
         <f>POINTS!K25</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I12" s="87">
         <f>POINTS!L25</f>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="J12" s="79"/>
     </row>
@@ -7532,15 +7529,15 @@
       </c>
       <c r="D13" s="85">
         <f>AVERAGE(3*E13,F13,G13,H13,I13)</f>
-        <v>12.8</v>
+        <v>14.8</v>
       </c>
       <c r="E13" s="86">
         <f>POINTS!H26</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F13" s="86">
         <f>POINTS!I26</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G13" s="86">
         <f>POINTS!J26</f>
@@ -7552,7 +7549,7 @@
       </c>
       <c r="I13" s="87">
         <f>POINTS!L26</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J13" s="79"/>
     </row>
@@ -7563,11 +7560,11 @@
       </c>
       <c r="C14" s="71">
         <f>RANK(D14,$D$3:$D$16,1)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D14" s="85">
         <f>AVERAGE(3*E14,F14,G14,H14,I14)</f>
-        <v>12.8</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="E14" s="86">
         <f>POINTS!H34</f>
@@ -7575,19 +7572,19 @@
       </c>
       <c r="F14" s="86">
         <f>POINTS!I34</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G14" s="86">
         <f>POINTS!J34</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H14" s="86">
         <f>POINTS!K34</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I14" s="87">
         <f>POINTS!L34</f>
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="J14" s="79"/>
     </row>
@@ -7598,15 +7595,15 @@
       </c>
       <c r="C15" s="71">
         <f>RANK(D15,$D$3:$D$16,1)</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="85">
         <f>AVERAGE(3*E15,F15,G15,H15,I15)</f>
-        <v>14.8</v>
+        <v>15.8</v>
       </c>
       <c r="E15" s="86">
         <f>POINTS!H23</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F15" s="86">
         <f>POINTS!I23</f>
@@ -7622,7 +7619,7 @@
       </c>
       <c r="I15" s="87">
         <f>POINTS!L23</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J15" s="79"/>
     </row>
@@ -7637,15 +7634,15 @@
       </c>
       <c r="D16" s="88">
         <f>AVERAGE(3*E16,F16,G16,H16,I16)</f>
-        <v>18.8</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="E16" s="89">
         <f>POINTS!H24</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F16" s="89">
         <f>POINTS!I24</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G16" s="89">
         <f>POINTS!J24</f>
@@ -7657,7 +7654,7 @@
       </c>
       <c r="I16" s="90">
         <f>POINTS!L24</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J16" s="80"/>
     </row>
@@ -7729,7 +7726,7 @@
       </c>
       <c r="D3" s="82">
         <f t="shared" ref="D3:D14" si="1">AVERAGE(3*E3,F3,G3,H3,I3)</f>
-        <v>1.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E3" s="83">
         <f>POINTS!H22</f>
@@ -7749,7 +7746,7 @@
       </c>
       <c r="I3" s="84">
         <f>POINTS!L22</f>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="J3" s="78"/>
     </row>
@@ -7764,11 +7761,11 @@
       </c>
       <c r="D4" s="85">
         <f t="shared" si="1"/>
-        <v>14.8</v>
+        <v>15.8</v>
       </c>
       <c r="E4" s="86">
         <f>POINTS!H23</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F4" s="86">
         <f>POINTS!I23</f>
@@ -7784,7 +7781,7 @@
       </c>
       <c r="I4" s="87">
         <f>POINTS!L23</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J4" s="79"/>
     </row>
@@ -7799,15 +7796,15 @@
       </c>
       <c r="D5" s="85">
         <f t="shared" si="1"/>
-        <v>18.8</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="E5" s="86">
         <f>POINTS!H24</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="86">
         <f>POINTS!I24</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="86">
         <f>POINTS!J24</f>
@@ -7819,7 +7816,7 @@
       </c>
       <c r="I5" s="87">
         <f>POINTS!L24</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J5" s="79"/>
     </row>
@@ -7834,7 +7831,7 @@
       </c>
       <c r="D6" s="85">
         <f t="shared" si="1"/>
-        <v>12.2</v>
+        <v>13</v>
       </c>
       <c r="E6" s="86">
         <f>POINTS!H25</f>
@@ -7842,19 +7839,19 @@
       </c>
       <c r="F6" s="86">
         <f>POINTS!I25</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G6" s="86">
         <f>POINTS!J25</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H6" s="86">
         <f>POINTS!K25</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I6" s="87">
         <f>POINTS!L25</f>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="J6" s="79"/>
     </row>
@@ -7869,15 +7866,15 @@
       </c>
       <c r="D7" s="85">
         <f t="shared" si="1"/>
-        <v>12.8</v>
+        <v>14.8</v>
       </c>
       <c r="E7" s="86">
         <f>POINTS!H26</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F7" s="86">
         <f>POINTS!I26</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="86">
         <f>POINTS!J26</f>
@@ -7889,7 +7886,7 @@
       </c>
       <c r="I7" s="87">
         <f>POINTS!L26</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J7" s="79"/>
     </row>
@@ -7900,19 +7897,19 @@
       </c>
       <c r="C8" s="71">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D8" s="85">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E8" s="86">
         <f>POINTS!H27</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F8" s="86">
         <f>POINTS!I27</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G8" s="86">
         <f>POINTS!J27</f>
@@ -7920,11 +7917,11 @@
       </c>
       <c r="H8" s="86">
         <f>POINTS!K27</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I8" s="87">
         <f>POINTS!L27</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J8" s="79"/>
     </row>
@@ -7935,19 +7932,19 @@
       </c>
       <c r="C9" s="71">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9" s="85">
         <f t="shared" si="1"/>
-        <v>4.5999999999999996</v>
+        <v>7</v>
       </c>
       <c r="E9" s="86">
         <f>POINTS!H28</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F9" s="86">
         <f>POINTS!I28</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G9" s="86">
         <f>POINTS!J28</f>
@@ -7959,7 +7956,7 @@
       </c>
       <c r="I9" s="87">
         <f>POINTS!L28</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J9" s="79"/>
     </row>
@@ -7974,11 +7971,11 @@
       </c>
       <c r="D10" s="85">
         <f t="shared" si="1"/>
-        <v>10.6</v>
+        <v>12</v>
       </c>
       <c r="E10" s="86">
         <f>POINTS!H29</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10" s="86">
         <f>POINTS!I29</f>
@@ -7986,15 +7983,15 @@
       </c>
       <c r="G10" s="86">
         <f>POINTS!J29</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H10" s="86">
         <f>POINTS!K29</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I10" s="87">
         <f>POINTS!L29</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J10" s="79"/>
     </row>
@@ -8005,19 +8002,19 @@
       </c>
       <c r="C11" s="71">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11" s="85">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>11.8</v>
       </c>
       <c r="E11" s="86">
         <f>POINTS!H30</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F11" s="86">
         <f>POINTS!I30</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G11" s="86">
         <f>POINTS!J30</f>
@@ -8025,11 +8022,11 @@
       </c>
       <c r="H11" s="86">
         <f>POINTS!K30</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I11" s="87">
         <f>POINTS!L30</f>
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="J11" s="79"/>
     </row>
@@ -8040,31 +8037,31 @@
       </c>
       <c r="C12" s="71">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D12" s="85">
         <f t="shared" si="1"/>
-        <v>7.4</v>
+        <v>11</v>
       </c>
       <c r="E12" s="86">
         <f>POINTS!H31</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F12" s="86">
         <f>POINTS!I31</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G12" s="86">
         <f>POINTS!J31</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H12" s="86">
         <f>POINTS!K31</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I12" s="87">
         <f>POINTS!L31</f>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="J12" s="79"/>
     </row>
@@ -8079,11 +8076,11 @@
       </c>
       <c r="D13" s="85">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E13" s="86">
         <f>POINTS!H32</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F13" s="86">
         <f>POINTS!I32</f>
@@ -8099,7 +8096,7 @@
       </c>
       <c r="I13" s="87">
         <f>POINTS!L32</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J13" s="79"/>
     </row>
@@ -8110,11 +8107,11 @@
       </c>
       <c r="C14" s="72">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="88">
         <f t="shared" si="1"/>
-        <v>5.2</v>
+        <v>6.6</v>
       </c>
       <c r="E14" s="89">
         <f>POINTS!H33</f>
@@ -8122,19 +8119,19 @@
       </c>
       <c r="F14" s="89">
         <f>POINTS!I33</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G14" s="89">
         <f>POINTS!J33</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H14" s="89">
         <f>POINTS!K33</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I14" s="90">
         <f>POINTS!L33</f>
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="J14" s="80"/>
     </row>
@@ -8206,7 +8203,7 @@
       </c>
       <c r="D3" s="83">
         <f t="shared" ref="D3:D12" si="1">AVERAGE(3*E3,F3,G3,H3,I3)</f>
-        <v>1.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E3" s="83">
         <f>POINTS!H22</f>
@@ -8226,7 +8223,7 @@
       </c>
       <c r="I3" s="83">
         <f>POINTS!L22</f>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="J3" s="73"/>
     </row>
@@ -8241,11 +8238,11 @@
       </c>
       <c r="D4" s="86">
         <f t="shared" si="1"/>
-        <v>14.8</v>
+        <v>15.8</v>
       </c>
       <c r="E4" s="86">
         <f>POINTS!H23</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F4" s="86">
         <f>POINTS!I23</f>
@@ -8261,7 +8258,7 @@
       </c>
       <c r="I4" s="86">
         <f>POINTS!L23</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J4" s="74"/>
     </row>
@@ -8276,15 +8273,15 @@
       </c>
       <c r="D5" s="86">
         <f t="shared" si="1"/>
-        <v>18.8</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="E5" s="86">
         <f>POINTS!H24</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="86">
         <f>POINTS!I24</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="86">
         <f>POINTS!J24</f>
@@ -8296,7 +8293,7 @@
       </c>
       <c r="I5" s="86">
         <f>POINTS!L24</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J5" s="74"/>
     </row>
@@ -8311,7 +8308,7 @@
       </c>
       <c r="D6" s="86">
         <f t="shared" si="1"/>
-        <v>12.2</v>
+        <v>13</v>
       </c>
       <c r="E6" s="86">
         <f>POINTS!H25</f>
@@ -8319,19 +8316,19 @@
       </c>
       <c r="F6" s="86">
         <f>POINTS!I25</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G6" s="86">
         <f>POINTS!J25</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H6" s="86">
         <f>POINTS!K25</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I6" s="86">
         <f>POINTS!L25</f>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="J6" s="74"/>
     </row>
@@ -8346,15 +8343,15 @@
       </c>
       <c r="D7" s="86">
         <f t="shared" si="1"/>
-        <v>12.8</v>
+        <v>14.8</v>
       </c>
       <c r="E7" s="86">
         <f>POINTS!H26</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F7" s="86">
         <f>POINTS!I26</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="86">
         <f>POINTS!J26</f>
@@ -8366,7 +8363,7 @@
       </c>
       <c r="I7" s="86">
         <f>POINTS!L26</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J7" s="74"/>
     </row>
@@ -8377,19 +8374,19 @@
       </c>
       <c r="C8" s="97">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D8" s="86">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E8" s="86">
         <f>POINTS!H27</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F8" s="86">
         <f>POINTS!I27</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G8" s="86">
         <f>POINTS!J27</f>
@@ -8397,11 +8394,11 @@
       </c>
       <c r="H8" s="86">
         <f>POINTS!K27</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I8" s="86">
         <f>POINTS!L27</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J8" s="74"/>
     </row>
@@ -8416,15 +8413,15 @@
       </c>
       <c r="D9" s="86">
         <f t="shared" si="1"/>
-        <v>4.5999999999999996</v>
+        <v>7</v>
       </c>
       <c r="E9" s="86">
         <f>POINTS!H28</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F9" s="86">
         <f>POINTS!I28</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G9" s="86">
         <f>POINTS!J28</f>
@@ -8436,7 +8433,7 @@
       </c>
       <c r="I9" s="86">
         <f>POINTS!L28</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J9" s="74"/>
     </row>
@@ -8451,11 +8448,11 @@
       </c>
       <c r="D10" s="86">
         <f t="shared" si="1"/>
-        <v>10.6</v>
+        <v>12</v>
       </c>
       <c r="E10" s="86">
         <f>POINTS!H29</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10" s="86">
         <f>POINTS!I29</f>
@@ -8463,15 +8460,15 @@
       </c>
       <c r="G10" s="86">
         <f>POINTS!J29</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H10" s="86">
         <f>POINTS!K29</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I10" s="86">
         <f>POINTS!L29</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J10" s="74"/>
     </row>
@@ -8482,19 +8479,19 @@
       </c>
       <c r="C11" s="97">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D11" s="86">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>11.8</v>
       </c>
       <c r="E11" s="86">
         <f>POINTS!H30</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F11" s="86">
         <f>POINTS!I30</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G11" s="86">
         <f>POINTS!J30</f>
@@ -8502,11 +8499,11 @@
       </c>
       <c r="H11" s="86">
         <f>POINTS!K30</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I11" s="86">
         <f>POINTS!L30</f>
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="J11" s="74"/>
     </row>
@@ -8517,31 +8514,31 @@
       </c>
       <c r="C12" s="99">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D12" s="89">
         <f t="shared" si="1"/>
-        <v>7.4</v>
+        <v>11</v>
       </c>
       <c r="E12" s="89">
         <f>POINTS!H31</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F12" s="89">
         <f>POINTS!I31</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G12" s="89">
         <f>POINTS!J31</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H12" s="89">
         <f>POINTS!K31</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I12" s="89">
         <f>POINTS!L31</f>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="J12" s="75"/>
     </row>
@@ -8613,7 +8610,7 @@
       </c>
       <c r="D3" s="82">
         <f t="shared" ref="D3:D10" si="1">AVERAGE(3*E3,F3,G3,H3,I3)</f>
-        <v>1.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E3" s="83">
         <f>POINTS!H22</f>
@@ -8633,7 +8630,7 @@
       </c>
       <c r="I3" s="84">
         <f>POINTS!L22</f>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="J3" s="78"/>
     </row>
@@ -8648,11 +8645,11 @@
       </c>
       <c r="D4" s="85">
         <f t="shared" si="1"/>
-        <v>14.8</v>
+        <v>15.8</v>
       </c>
       <c r="E4" s="86">
         <f>POINTS!H23</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F4" s="86">
         <f>POINTS!I23</f>
@@ -8668,7 +8665,7 @@
       </c>
       <c r="I4" s="87">
         <f>POINTS!L23</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J4" s="79"/>
     </row>
@@ -8683,15 +8680,15 @@
       </c>
       <c r="D5" s="85">
         <f t="shared" si="1"/>
-        <v>18.8</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="E5" s="86">
         <f>POINTS!H24</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="86">
         <f>POINTS!I24</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="86">
         <f>POINTS!J24</f>
@@ -8703,7 +8700,7 @@
       </c>
       <c r="I5" s="87">
         <f>POINTS!L24</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J5" s="79"/>
     </row>
@@ -8718,7 +8715,7 @@
       </c>
       <c r="D6" s="85">
         <f t="shared" si="1"/>
-        <v>12.2</v>
+        <v>13</v>
       </c>
       <c r="E6" s="86">
         <f>POINTS!H25</f>
@@ -8726,19 +8723,19 @@
       </c>
       <c r="F6" s="86">
         <f>POINTS!I25</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G6" s="86">
         <f>POINTS!J25</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H6" s="86">
         <f>POINTS!K25</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I6" s="87">
         <f>POINTS!L25</f>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="J6" s="79"/>
     </row>
@@ -8753,15 +8750,15 @@
       </c>
       <c r="D7" s="85">
         <f t="shared" si="1"/>
-        <v>12.8</v>
+        <v>14.8</v>
       </c>
       <c r="E7" s="86">
         <f>POINTS!H26</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F7" s="86">
         <f>POINTS!I26</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="86">
         <f>POINTS!J26</f>
@@ -8773,7 +8770,7 @@
       </c>
       <c r="I7" s="87">
         <f>POINTS!L26</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J7" s="79"/>
     </row>
@@ -8788,15 +8785,15 @@
       </c>
       <c r="D8" s="85">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E8" s="86">
         <f>POINTS!H27</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F8" s="86">
         <f>POINTS!I27</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G8" s="86">
         <f>POINTS!J27</f>
@@ -8804,11 +8801,11 @@
       </c>
       <c r="H8" s="86">
         <f>POINTS!K27</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I8" s="87">
         <f>POINTS!L27</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J8" s="79"/>
     </row>
@@ -8823,15 +8820,15 @@
       </c>
       <c r="D9" s="85">
         <f t="shared" si="1"/>
-        <v>4.5999999999999996</v>
+        <v>7</v>
       </c>
       <c r="E9" s="86">
         <f>POINTS!H28</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F9" s="86">
         <f>POINTS!I28</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G9" s="86">
         <f>POINTS!J28</f>
@@ -8843,7 +8840,7 @@
       </c>
       <c r="I9" s="87">
         <f>POINTS!L28</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J9" s="79"/>
     </row>
@@ -8858,11 +8855,11 @@
       </c>
       <c r="D10" s="88">
         <f t="shared" si="1"/>
-        <v>10.6</v>
+        <v>12</v>
       </c>
       <c r="E10" s="89">
         <f>POINTS!H29</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10" s="89">
         <f>POINTS!I29</f>
@@ -8870,15 +8867,15 @@
       </c>
       <c r="G10" s="89">
         <f>POINTS!J29</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H10" s="89">
         <f>POINTS!K29</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I10" s="90">
         <f>POINTS!L29</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J10" s="80"/>
     </row>

</xml_diff>

<commit_message>
End of Season Rankings
</commit_message>
<xml_diff>
--- a/Power Rankings.xlsx
+++ b/Power Rankings.xlsx
@@ -3618,7 +3618,7 @@
   <dimension ref="A1:AO44"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3803,14 +3803,16 @@
       <c r="N3" s="7">
         <v>106.7</v>
       </c>
-      <c r="O3" s="8"/>
+      <c r="O3" s="8">
+        <v>128.69999999999999</v>
+      </c>
       <c r="P3" s="12">
         <f>SUM(C3:O3)</f>
-        <v>1329.1000000000001</v>
+        <v>1457.8000000000002</v>
       </c>
       <c r="Q3" s="12">
         <f>AVERAGE(C3:O3)</f>
-        <v>110.75833333333334</v>
+        <v>112.13846153846156</v>
       </c>
       <c r="R3" s="13">
         <f>MAX(C3:O3)</f>
@@ -3822,7 +3824,7 @@
       </c>
       <c r="T3" s="13">
         <f>STDEV(C3:O3)</f>
-        <v>15.54684758068241</v>
+        <v>15.694719837232903</v>
       </c>
       <c r="W3" s="52">
         <f>IF(C3="","",RANK(C3,$C$3:$C$18,1))</f>
@@ -3872,13 +3874,13 @@
         <f>IF(N3="","",RANK(N3,$N$3:$N$18,1))</f>
         <v>9</v>
       </c>
-      <c r="AI3" s="54" t="str">
+      <c r="AI3" s="54">
         <f>IF(O3="","",RANK(O3,$O$3:$O$18,1))</f>
-        <v/>
+        <v>13</v>
       </c>
       <c r="AJ3" s="42">
         <f>SUM(W3:AI3)</f>
-        <v>117</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3924,14 +3926,16 @@
       <c r="N4" s="34">
         <v>93.3</v>
       </c>
-      <c r="O4" s="9"/>
+      <c r="O4" s="9">
+        <v>99.3</v>
+      </c>
       <c r="P4" s="14">
         <f t="shared" ref="P4:P18" si="0">SUM(C4:O4)</f>
-        <v>1072.3</v>
+        <v>1171.5999999999999</v>
       </c>
       <c r="Q4" s="14">
         <f t="shared" ref="Q4:Q18" si="1">AVERAGE(C4:O4)</f>
-        <v>89.358333333333334</v>
+        <v>90.123076923076923</v>
       </c>
       <c r="R4" s="15">
         <f t="shared" ref="R4:R18" si="2">MAX(C4:O4)</f>
@@ -3943,7 +3947,7 @@
       </c>
       <c r="T4" s="15">
         <f t="shared" ref="T4:T18" si="4">STDEV(C4:O4)</f>
-        <v>20.802336334404824</v>
+        <v>20.106680226819943</v>
       </c>
       <c r="W4" s="55">
         <f t="shared" ref="W4:W18" si="5">IF(C4="","",RANK(C4,$C$3:$C$18,1))</f>
@@ -3993,13 +3997,13 @@
         <f t="shared" ref="AH4:AH18" si="16">IF(N4="","",RANK(N4,$N$3:$N$18,1))</f>
         <v>6</v>
       </c>
-      <c r="AI4" s="57" t="str">
+      <c r="AI4" s="57">
         <f t="shared" ref="AI4:AI18" si="17">IF(O4="","",RANK(O4,$O$3:$O$18,1))</f>
-        <v/>
+        <v>9</v>
       </c>
       <c r="AJ4" s="43">
         <f t="shared" ref="AJ4:AJ18" si="18">SUM(W4:AI4)</f>
-        <v>64</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4045,14 +4049,16 @@
       <c r="N5" s="36">
         <v>113.5</v>
       </c>
-      <c r="O5" s="8"/>
+      <c r="O5" s="8">
+        <v>74.8</v>
+      </c>
       <c r="P5" s="16">
         <f t="shared" si="0"/>
-        <v>991.20000000000016</v>
+        <v>1066.0000000000002</v>
       </c>
       <c r="Q5" s="16">
         <f t="shared" si="1"/>
-        <v>82.600000000000009</v>
+        <v>82.000000000000014</v>
       </c>
       <c r="R5" s="17">
         <f t="shared" si="2"/>
@@ -4064,7 +4070,7 @@
       </c>
       <c r="T5" s="17">
         <f t="shared" si="4"/>
-        <v>19.825786697677756</v>
+        <v>19.104624222074193</v>
       </c>
       <c r="W5" s="55">
         <f t="shared" si="5"/>
@@ -4114,13 +4120,13 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AI5" s="57" t="str">
+      <c r="AI5" s="57">
         <f t="shared" si="17"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AJ5" s="43">
         <f t="shared" si="18"/>
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4166,14 +4172,16 @@
       <c r="N6" s="34">
         <v>79.400000000000006</v>
       </c>
-      <c r="O6" s="9"/>
+      <c r="O6" s="9">
+        <v>80.2</v>
+      </c>
       <c r="P6" s="14">
         <f t="shared" si="0"/>
-        <v>1166.0000000000002</v>
+        <v>1246.2000000000003</v>
       </c>
       <c r="Q6" s="14">
         <f t="shared" si="1"/>
-        <v>97.166666666666686</v>
+        <v>95.861538461538487</v>
       </c>
       <c r="R6" s="15">
         <f t="shared" si="2"/>
@@ -4185,7 +4193,7 @@
       </c>
       <c r="T6" s="15">
         <f t="shared" si="4"/>
-        <v>15.105527786110821</v>
+        <v>15.208744111066295</v>
       </c>
       <c r="W6" s="55">
         <f t="shared" si="5"/>
@@ -4235,13 +4243,13 @@
         <f t="shared" si="16"/>
         <v>4</v>
       </c>
-      <c r="AI6" s="57" t="str">
+      <c r="AI6" s="57">
         <f t="shared" si="17"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="AJ6" s="43">
         <f t="shared" si="18"/>
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4287,14 +4295,16 @@
       <c r="N7" s="36">
         <v>77.900000000000006</v>
       </c>
-      <c r="O7" s="8"/>
+      <c r="O7" s="8">
+        <v>86.6</v>
+      </c>
       <c r="P7" s="16">
         <f t="shared" si="0"/>
-        <v>1152.9000000000001</v>
+        <v>1239.5</v>
       </c>
       <c r="Q7" s="16">
         <f t="shared" si="1"/>
-        <v>96.075000000000003</v>
+        <v>95.34615384615384</v>
       </c>
       <c r="R7" s="17">
         <f t="shared" si="2"/>
@@ -4306,7 +4316,7 @@
       </c>
       <c r="T7" s="17">
         <f t="shared" si="4"/>
-        <v>20.657383667831677</v>
+        <v>19.95175912814938</v>
       </c>
       <c r="W7" s="55">
         <f t="shared" si="5"/>
@@ -4356,13 +4366,13 @@
         <f t="shared" si="16"/>
         <v>2</v>
       </c>
-      <c r="AI7" s="57" t="str">
+      <c r="AI7" s="57">
         <f t="shared" si="17"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="AJ7" s="43">
         <f t="shared" si="18"/>
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4408,14 +4418,16 @@
       <c r="N8" s="34">
         <v>79.3</v>
       </c>
-      <c r="O8" s="9"/>
+      <c r="O8" s="9">
+        <v>81.400000000000006</v>
+      </c>
       <c r="P8" s="14">
         <f t="shared" si="0"/>
-        <v>1201.3</v>
+        <v>1282.7</v>
       </c>
       <c r="Q8" s="14">
         <f t="shared" si="1"/>
-        <v>100.10833333333333</v>
+        <v>98.669230769230779</v>
       </c>
       <c r="R8" s="15">
         <f t="shared" si="2"/>
@@ -4427,7 +4439,7 @@
       </c>
       <c r="T8" s="15">
         <f t="shared" si="4"/>
-        <v>22.589637943629018</v>
+        <v>22.241642048770597</v>
       </c>
       <c r="W8" s="55">
         <f t="shared" si="5"/>
@@ -4477,13 +4489,13 @@
         <f t="shared" si="16"/>
         <v>3</v>
       </c>
-      <c r="AI8" s="57" t="str">
+      <c r="AI8" s="57">
         <f t="shared" si="17"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="AJ8" s="43">
         <f t="shared" si="18"/>
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4529,14 +4541,16 @@
       <c r="N9" s="36">
         <v>128.30000000000001</v>
       </c>
-      <c r="O9" s="8"/>
+      <c r="O9" s="8">
+        <v>86.2</v>
+      </c>
       <c r="P9" s="16">
         <f t="shared" si="0"/>
-        <v>1346.4</v>
+        <v>1432.6000000000001</v>
       </c>
       <c r="Q9" s="16">
         <f t="shared" si="1"/>
-        <v>112.2</v>
+        <v>110.20000000000002</v>
       </c>
       <c r="R9" s="17">
         <f t="shared" si="2"/>
@@ -4548,7 +4562,7 @@
       </c>
       <c r="T9" s="17">
         <f t="shared" si="4"/>
-        <v>23.535350587419089</v>
+        <v>23.659106773784416</v>
       </c>
       <c r="W9" s="55">
         <f t="shared" si="5"/>
@@ -4598,13 +4612,13 @@
         <f t="shared" si="16"/>
         <v>13</v>
       </c>
-      <c r="AI9" s="57" t="str">
+      <c r="AI9" s="57">
         <f t="shared" si="17"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="AJ9" s="43">
         <f t="shared" si="18"/>
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4650,14 +4664,16 @@
       <c r="N10" s="34">
         <v>89.5</v>
       </c>
-      <c r="O10" s="9"/>
+      <c r="O10" s="9">
+        <v>131.69999999999999</v>
+      </c>
       <c r="P10" s="14">
         <f t="shared" si="0"/>
-        <v>1266.5</v>
+        <v>1398.2</v>
       </c>
       <c r="Q10" s="14">
         <f t="shared" si="1"/>
-        <v>105.54166666666667</v>
+        <v>107.55384615384615</v>
       </c>
       <c r="R10" s="15">
         <f t="shared" si="2"/>
@@ -4669,7 +4685,7 @@
       </c>
       <c r="T10" s="15">
         <f t="shared" si="4"/>
-        <v>21.828565868576582</v>
+        <v>22.12271138387781</v>
       </c>
       <c r="W10" s="55">
         <f t="shared" si="5"/>
@@ -4719,13 +4735,13 @@
         <f t="shared" si="16"/>
         <v>5</v>
       </c>
-      <c r="AI10" s="57" t="str">
+      <c r="AI10" s="57">
         <f t="shared" si="17"/>
-        <v/>
+        <v>14</v>
       </c>
       <c r="AJ10" s="43">
         <f t="shared" si="18"/>
-        <v>99</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4771,14 +4787,16 @@
       <c r="N11" s="36">
         <v>98</v>
       </c>
-      <c r="O11" s="8"/>
+      <c r="O11" s="8">
+        <v>88.7</v>
+      </c>
       <c r="P11" s="16">
         <f t="shared" si="0"/>
-        <v>1151.3999999999999</v>
+        <v>1240.0999999999999</v>
       </c>
       <c r="Q11" s="16">
         <f t="shared" si="1"/>
-        <v>95.949999999999989</v>
+        <v>95.392307692307682</v>
       </c>
       <c r="R11" s="17">
         <f t="shared" si="2"/>
@@ -4790,7 +4808,7 @@
       </c>
       <c r="T11" s="17">
         <f t="shared" si="4"/>
-        <v>26.032619398118108</v>
+        <v>25.005314819669248</v>
       </c>
       <c r="W11" s="55">
         <f t="shared" si="5"/>
@@ -4840,13 +4858,13 @@
         <f t="shared" si="16"/>
         <v>7</v>
       </c>
-      <c r="AI11" s="57" t="str">
+      <c r="AI11" s="57">
         <f t="shared" si="17"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="AJ11" s="43">
         <f t="shared" si="18"/>
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4892,14 +4910,16 @@
       <c r="N12" s="34">
         <v>75.599999999999994</v>
       </c>
-      <c r="O12" s="9"/>
+      <c r="O12" s="9">
+        <v>97.8</v>
+      </c>
       <c r="P12" s="14">
         <f t="shared" ref="P12:P17" si="19">SUM(C12:O12)</f>
-        <v>1161.3</v>
+        <v>1259.0999999999999</v>
       </c>
       <c r="Q12" s="14">
         <f t="shared" ref="Q12:Q17" si="20">AVERAGE(C12:O12)</f>
-        <v>96.774999999999991</v>
+        <v>96.853846153846149</v>
       </c>
       <c r="R12" s="15">
         <f t="shared" ref="R12:R17" si="21">MAX(C12:O12)</f>
@@ -4911,7 +4931,7 @@
       </c>
       <c r="T12" s="15">
         <f t="shared" ref="T12:T17" si="23">STDEV(C12:O12)</f>
-        <v>21.073987628008499</v>
+        <v>20.178809652067184</v>
       </c>
       <c r="W12" s="55">
         <f t="shared" si="5"/>
@@ -4961,13 +4981,13 @@
         <f t="shared" si="16"/>
         <v>1</v>
       </c>
-      <c r="AI12" s="57" t="str">
+      <c r="AI12" s="57">
         <f t="shared" si="17"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="AJ12" s="43">
         <f t="shared" si="18"/>
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5013,14 +5033,16 @@
       <c r="N13" s="36">
         <v>111.1</v>
       </c>
-      <c r="O13" s="8"/>
+      <c r="O13" s="8">
+        <v>96.1</v>
+      </c>
       <c r="P13" s="16">
         <f t="shared" si="19"/>
-        <v>1229.9000000000001</v>
+        <v>1326</v>
       </c>
       <c r="Q13" s="16">
         <f t="shared" si="20"/>
-        <v>102.49166666666667</v>
+        <v>102</v>
       </c>
       <c r="R13" s="17">
         <f t="shared" si="21"/>
@@ -5032,7 +5054,7 @@
       </c>
       <c r="T13" s="17">
         <f t="shared" si="23"/>
-        <v>19.533396033615315</v>
+        <v>18.785632808079662</v>
       </c>
       <c r="W13" s="55">
         <f t="shared" si="5"/>
@@ -5082,13 +5104,13 @@
         <f t="shared" si="16"/>
         <v>10</v>
       </c>
-      <c r="AI13" s="57" t="str">
+      <c r="AI13" s="57">
         <f t="shared" si="17"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="AJ13" s="43">
         <f t="shared" si="18"/>
-        <v>94</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5134,14 +5156,16 @@
       <c r="N14" s="34">
         <v>139.6</v>
       </c>
-      <c r="O14" s="9"/>
+      <c r="O14" s="9">
+        <v>107.7</v>
+      </c>
       <c r="P14" s="14">
         <f t="shared" si="19"/>
-        <v>1353.4999999999998</v>
+        <v>1461.1999999999998</v>
       </c>
       <c r="Q14" s="14">
         <f t="shared" si="20"/>
-        <v>112.79166666666664</v>
+        <v>112.39999999999999</v>
       </c>
       <c r="R14" s="15">
         <f t="shared" si="21"/>
@@ -5153,7 +5177,7 @@
       </c>
       <c r="T14" s="15">
         <f t="shared" si="23"/>
-        <v>20.633444093304483</v>
+        <v>19.805428548759227</v>
       </c>
       <c r="W14" s="55">
         <f t="shared" si="5"/>
@@ -5203,13 +5227,13 @@
         <f t="shared" si="16"/>
         <v>14</v>
       </c>
-      <c r="AI14" s="57" t="str">
+      <c r="AI14" s="57">
         <f t="shared" si="17"/>
-        <v/>
+        <v>10</v>
       </c>
       <c r="AJ14" s="43">
         <f t="shared" si="18"/>
-        <v>115</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5255,14 +5279,16 @@
       <c r="N15" s="36">
         <v>111.4</v>
       </c>
-      <c r="O15" s="8"/>
+      <c r="O15" s="8">
+        <v>111.4</v>
+      </c>
       <c r="P15" s="16">
         <f t="shared" si="19"/>
-        <v>1170.2000000000003</v>
+        <v>1281.6000000000004</v>
       </c>
       <c r="Q15" s="16">
         <f t="shared" si="20"/>
-        <v>97.516666666666694</v>
+        <v>98.584615384615418</v>
       </c>
       <c r="R15" s="17">
         <f t="shared" si="21"/>
@@ -5274,7 +5300,7 @@
       </c>
       <c r="T15" s="17">
         <f t="shared" si="23"/>
-        <v>13.133152590665052</v>
+        <v>13.150402158225916</v>
       </c>
       <c r="W15" s="55">
         <f t="shared" si="5"/>
@@ -5324,13 +5350,13 @@
         <f t="shared" si="16"/>
         <v>11</v>
       </c>
-      <c r="AI15" s="57" t="str">
+      <c r="AI15" s="57">
         <f t="shared" si="17"/>
-        <v/>
+        <v>11</v>
       </c>
       <c r="AJ15" s="43">
         <f t="shared" si="18"/>
-        <v>83</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:36" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5376,14 +5402,16 @@
       <c r="N16" s="34">
         <v>103.4</v>
       </c>
-      <c r="O16" s="9"/>
+      <c r="O16" s="9">
+        <v>111.4</v>
+      </c>
       <c r="P16" s="14">
         <f t="shared" si="19"/>
-        <v>1186.2</v>
+        <v>1297.6000000000001</v>
       </c>
       <c r="Q16" s="14">
         <f t="shared" si="20"/>
-        <v>98.850000000000009</v>
+        <v>99.81538461538463</v>
       </c>
       <c r="R16" s="15">
         <f t="shared" si="21"/>
@@ -5395,7 +5423,7 @@
       </c>
       <c r="T16" s="15">
         <f t="shared" si="23"/>
-        <v>25.670694292413369</v>
+        <v>24.823068778653099</v>
       </c>
       <c r="W16" s="55">
         <f t="shared" si="5"/>
@@ -5445,13 +5473,13 @@
         <f t="shared" si="16"/>
         <v>8</v>
       </c>
-      <c r="AI16" s="57" t="str">
+      <c r="AI16" s="57">
         <f t="shared" si="17"/>
-        <v/>
+        <v>11</v>
       </c>
       <c r="AJ16" s="43">
         <f t="shared" si="18"/>
-        <v>91</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:41" ht="24" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5647,11 +5675,11 @@
     <row r="19" spans="1:41" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P19" s="11">
         <f>SUM(C3:O18)</f>
-        <v>16778.2</v>
+        <v>18160.200000000008</v>
       </c>
       <c r="Q19" s="11">
         <f>AVERAGE(C3:O18)</f>
-        <v>99.870238095238093</v>
+        <v>99.781318681318723</v>
       </c>
       <c r="R19" s="18">
         <f>MAX(C3:O18)</f>
@@ -5663,7 +5691,7 @@
       </c>
       <c r="T19" s="18">
         <f>STDEV(C3:O18)</f>
-        <v>21.545652852238948</v>
+        <v>21.227147801254858</v>
       </c>
     </row>
     <row r="20" spans="1:41" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -5718,23 +5746,21 @@
         <v>Spos Before Hos</v>
       </c>
       <c r="C22" s="21">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D22" s="46">
         <f>AJ3</f>
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="E22" s="49">
         <f t="shared" ref="E22:E31" si="24">IF(D3="",-99,IF(T3=0,1,(Q3-$Q$19)/T3))</f>
-        <v>0.70034102936881859</v>
+        <v>0.78734395932495282</v>
       </c>
       <c r="F22" s="28">
         <f>IF(C3="",0,Q3)</f>
-        <v>110.75833333333334</v>
-      </c>
-      <c r="G22" s="39">
-        <v>100</v>
-      </c>
+        <v>112.13846153846156</v>
+      </c>
+      <c r="G22" s="39"/>
       <c r="H22" s="22">
         <f>IF(C22="",16,RANK(C22,$C$22:$C$37,0))</f>
         <v>1</v>
@@ -5749,11 +5775,11 @@
       </c>
       <c r="K22" s="22">
         <f>IF(C22="",16,RANK(F22,$F$22:$F$37,0))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L22" s="22">
         <f t="shared" ref="L22" si="25">IF(G22="",16,RANK(G22,$G$22:$G$37,0))</f>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="N22" s="104"/>
       <c r="O22" s="104"/>
@@ -5775,19 +5801,17 @@
       </c>
       <c r="D23" s="47">
         <f t="shared" ref="D23:D37" si="26">AJ4</f>
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="E23" s="50">
         <f t="shared" si="24"/>
-        <v>-0.50532327681478739</v>
+        <v>-0.48034989611854689</v>
       </c>
       <c r="F23" s="28">
         <f t="shared" ref="F23:F37" si="27">IF(C4="",0,Q4)</f>
-        <v>89.358333333333334</v>
-      </c>
-      <c r="G23" s="40">
-        <v>86.9</v>
-      </c>
+        <v>90.123076923076923</v>
+      </c>
+      <c r="G23" s="40"/>
       <c r="H23" s="24">
         <f t="shared" ref="H23:H37" si="28">IF(C23="",16,RANK(C23,$C$22:$C$37,0))</f>
         <v>7</v>
@@ -5806,7 +5830,7 @@
       </c>
       <c r="L23" s="24">
         <f t="shared" ref="L23:L37" si="31">IF(G23="",16,RANK(G23,$G$22:$G$37,0))</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="N23" s="30"/>
       <c r="O23" s="30"/>
@@ -5824,19 +5848,17 @@
       </c>
       <c r="D24" s="47">
         <f t="shared" si="26"/>
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E24" s="50">
         <f t="shared" si="24"/>
-        <v>-0.87109976308082604</v>
+        <v>-0.93073375715883022</v>
       </c>
       <c r="F24" s="28">
         <f t="shared" si="27"/>
-        <v>82.600000000000009</v>
-      </c>
-      <c r="G24" s="40">
-        <v>76.099999999999994</v>
-      </c>
+        <v>82.000000000000014</v>
+      </c>
+      <c r="G24" s="40"/>
       <c r="H24" s="24">
         <f t="shared" si="28"/>
         <v>14</v>
@@ -5855,7 +5877,7 @@
       </c>
       <c r="L24" s="24">
         <f t="shared" si="31"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="N24" s="104" t="s">
         <v>44</v>
@@ -5885,38 +5907,36 @@
       </c>
       <c r="D25" s="47">
         <f t="shared" si="26"/>
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E25" s="50">
         <f t="shared" si="24"/>
-        <v>-0.17897894511552773</v>
+        <v>-0.25773201200275947</v>
       </c>
       <c r="F25" s="28">
         <f t="shared" si="27"/>
-        <v>97.166666666666686</v>
-      </c>
-      <c r="G25" s="40">
-        <v>71.8</v>
-      </c>
+        <v>95.861538461538487</v>
+      </c>
+      <c r="G25" s="40"/>
       <c r="H25" s="24">
         <f t="shared" si="28"/>
         <v>8</v>
       </c>
       <c r="I25" s="24">
         <f t="shared" si="29"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J25" s="24">
         <f>RANK(E25,$E$22:$E40,0)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K25" s="24">
         <f t="shared" si="30"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L25" s="24">
         <f t="shared" si="31"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N25" s="104"/>
       <c r="O25" s="104"/>
@@ -5944,38 +5964,36 @@
       </c>
       <c r="D26" s="47">
         <f t="shared" si="26"/>
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="E26" s="50">
         <f t="shared" si="24"/>
-        <v>-0.18372307724274656</v>
+        <v>-0.22229442560317567</v>
       </c>
       <c r="F26" s="28">
         <f t="shared" si="27"/>
-        <v>96.075000000000003</v>
-      </c>
-      <c r="G26" s="40">
-        <v>82.7</v>
-      </c>
+        <v>95.34615384615384</v>
+      </c>
+      <c r="G26" s="40"/>
       <c r="H26" s="24">
         <f t="shared" si="28"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I26" s="24">
         <f t="shared" si="29"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J26" s="24">
         <f>RANK(E26,$E$22:$E41,0)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K26" s="24">
         <f t="shared" si="30"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L26" s="24">
         <f t="shared" si="31"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="N26" s="30"/>
       <c r="O26" s="30"/>
@@ -5993,38 +6011,36 @@
       </c>
       <c r="D27" s="47">
         <f t="shared" si="26"/>
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E27" s="50">
         <f t="shared" si="24"/>
-        <v>1.054002010520895E-2</v>
+        <v>-5.0000261205957776E-2</v>
       </c>
       <c r="F27" s="28">
         <f t="shared" si="27"/>
-        <v>100.10833333333333</v>
-      </c>
-      <c r="G27" s="40">
-        <v>86.2</v>
-      </c>
+        <v>98.669230769230779</v>
+      </c>
+      <c r="G27" s="40"/>
       <c r="H27" s="24">
         <f t="shared" si="28"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I27" s="24">
         <f t="shared" si="29"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J27" s="24">
         <f>RANK(E27,$E$22:$E42,0)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K27" s="24">
         <f t="shared" si="30"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L27" s="24">
         <f t="shared" si="31"/>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="N27" s="100" t="s">
         <v>45</v>
@@ -6048,19 +6064,17 @@
       </c>
       <c r="D28" s="47">
         <f t="shared" si="26"/>
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E28" s="50">
         <f t="shared" si="24"/>
-        <v>0.52388265298893955</v>
+        <v>0.44036663844916424</v>
       </c>
       <c r="F28" s="28">
         <f t="shared" si="27"/>
-        <v>112.2</v>
-      </c>
-      <c r="G28" s="40">
-        <v>94.6</v>
-      </c>
+        <v>110.20000000000002</v>
+      </c>
+      <c r="G28" s="40"/>
       <c r="H28" s="24">
         <f t="shared" si="28"/>
         <v>3</v>
@@ -6075,11 +6089,11 @@
       </c>
       <c r="K28" s="24">
         <f t="shared" si="30"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L28" s="24">
         <f t="shared" si="31"/>
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="N28" s="100"/>
       <c r="O28" s="100"/>
@@ -6097,26 +6111,24 @@
         <v>Team Wasserman</v>
       </c>
       <c r="C29" s="23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D29" s="47">
         <f t="shared" si="26"/>
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E29" s="50">
         <f t="shared" si="24"/>
-        <v>0.25981682010511331</v>
+        <v>0.35133701912287979</v>
       </c>
       <c r="F29" s="28">
         <f t="shared" si="27"/>
-        <v>105.54166666666667</v>
-      </c>
-      <c r="G29" s="40">
-        <v>84.9</v>
-      </c>
+        <v>107.55384615384615</v>
+      </c>
+      <c r="G29" s="40"/>
       <c r="H29" s="24">
         <f t="shared" si="28"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I29" s="24">
         <f t="shared" si="29"/>
@@ -6132,7 +6144,7 @@
       </c>
       <c r="L29" s="24">
         <f t="shared" si="31"/>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="N29" s="100"/>
       <c r="O29" s="100"/>
@@ -6154,19 +6166,17 @@
       </c>
       <c r="D30" s="47">
         <f t="shared" si="26"/>
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E30" s="50">
         <f t="shared" si="24"/>
-        <v>-0.15058945991126418</v>
+        <v>-0.17552312461023817</v>
       </c>
       <c r="F30" s="28">
         <f t="shared" si="27"/>
-        <v>95.949999999999989</v>
-      </c>
-      <c r="G30" s="40">
-        <v>83.3</v>
-      </c>
+        <v>95.392307692307682</v>
+      </c>
+      <c r="G30" s="40"/>
       <c r="H30" s="24">
         <f t="shared" si="28"/>
         <v>8</v>
@@ -6177,15 +6187,15 @@
       </c>
       <c r="J30" s="24">
         <f>RANK(E30,$E$22:$E45,0)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K30" s="24">
         <f t="shared" si="30"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L30" s="24">
         <f t="shared" si="31"/>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="N30" s="100"/>
       <c r="O30" s="100"/>
@@ -6203,42 +6213,40 @@
         <v>Team Frisch</v>
       </c>
       <c r="C31" s="23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D31" s="47">
         <f t="shared" si="26"/>
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E31" s="50">
         <f t="shared" si="24"/>
-        <v>-0.14687481789750881</v>
+        <v>-0.14507657180723116</v>
       </c>
       <c r="F31" s="28">
         <f t="shared" si="27"/>
-        <v>96.774999999999991</v>
-      </c>
-      <c r="G31" s="40">
-        <v>84.6</v>
-      </c>
+        <v>96.853846153846149</v>
+      </c>
+      <c r="G31" s="40"/>
       <c r="H31" s="24">
         <f t="shared" si="28"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I31" s="24">
         <f t="shared" si="29"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J31" s="24">
         <f>RANK(E31,$E$22:$E46,0)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K31" s="24">
         <f t="shared" si="30"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L31" s="24">
         <f t="shared" si="31"/>
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="N31" s="100"/>
       <c r="O31" s="100"/>
@@ -6256,23 +6264,21 @@
         <v>OhNo Romo</v>
       </c>
       <c r="C32" s="23">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D32" s="47">
         <f t="shared" si="26"/>
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="E32" s="50">
         <f>IF(D13="",-99,IF(T13=0,1,(Q13-$Q$19)/T13))</f>
-        <v>0.13420239711094401</v>
+        <v>0.11810522122667205</v>
       </c>
       <c r="F32" s="28">
         <f t="shared" si="27"/>
-        <v>102.49166666666667</v>
-      </c>
-      <c r="G32" s="40">
-        <v>69.099999999999994</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="G32" s="40"/>
       <c r="H32" s="24">
         <f t="shared" si="28"/>
         <v>4</v>
@@ -6291,7 +6297,7 @@
       </c>
       <c r="L32" s="24">
         <f t="shared" si="31"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="N32" s="77"/>
       <c r="O32" s="77"/>
@@ -6309,23 +6315,21 @@
         <v>Cool Hand Lou</v>
       </c>
       <c r="C33" s="23">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D33" s="47">
         <f t="shared" si="26"/>
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="E33" s="50">
         <f t="shared" ref="E33:E37" si="32">IF(D14="",-99,IF(T14=0,1,(Q14-$Q$19)/T14))</f>
-        <v>0.62623711838885543</v>
+        <v>0.63713245525665763</v>
       </c>
       <c r="F33" s="28">
         <f t="shared" si="27"/>
-        <v>112.79166666666664</v>
-      </c>
-      <c r="G33" s="40">
-        <v>94.7</v>
-      </c>
+        <v>112.39999999999999</v>
+      </c>
+      <c r="G33" s="40"/>
       <c r="H33" s="24">
         <f t="shared" si="28"/>
         <v>2</v>
@@ -6344,7 +6348,7 @@
       </c>
       <c r="L33" s="24">
         <f t="shared" si="31"/>
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="N33" s="100" t="s">
         <v>47</v>
@@ -6364,34 +6368,32 @@
         <v>Hebrew Wolves</v>
       </c>
       <c r="C34" s="23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D34" s="47">
         <f t="shared" si="26"/>
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="E34" s="50">
         <f t="shared" si="32"/>
-        <v>-0.17920841262777229</v>
+        <v>-9.1001269946313856E-2</v>
       </c>
       <c r="F34" s="28">
         <f t="shared" si="27"/>
-        <v>97.516666666666694</v>
-      </c>
-      <c r="G34" s="40">
-        <v>83.8</v>
-      </c>
+        <v>98.584615384615418</v>
+      </c>
+      <c r="G34" s="40"/>
       <c r="H34" s="24">
         <f t="shared" si="28"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I34" s="24">
         <f t="shared" si="29"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J34" s="24">
         <f>RANK(E34,$E$22:$E49,0)</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="K34" s="24">
         <f t="shared" si="30"/>
@@ -6399,7 +6401,7 @@
       </c>
       <c r="L34" s="24">
         <f t="shared" si="31"/>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="N34" s="100"/>
       <c r="O34" s="100"/>
@@ -6417,42 +6419,40 @@
         <v>Team Force</v>
       </c>
       <c r="C35" s="23">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D35" s="47">
         <f t="shared" si="26"/>
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="E35" s="50">
         <f t="shared" si="32"/>
-        <v>-3.974329964030629E-2</v>
+        <v>1.3723498238542818E-3</v>
       </c>
       <c r="F35" s="28">
         <f t="shared" si="27"/>
-        <v>98.850000000000009</v>
-      </c>
-      <c r="G35" s="40">
-        <v>84.5</v>
-      </c>
+        <v>99.81538461538463</v>
+      </c>
+      <c r="G35" s="40"/>
       <c r="H35" s="24">
         <f t="shared" si="28"/>
         <v>4</v>
       </c>
       <c r="I35" s="24">
         <f t="shared" si="29"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J35" s="24">
         <f>RANK(E35,$E$22:$E50,0)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K35" s="24">
         <f t="shared" si="30"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L35" s="24">
         <f t="shared" si="31"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="N35" s="100"/>
       <c r="O35" s="100"/>
@@ -6718,7 +6718,7 @@
       </c>
       <c r="D3" s="82">
         <f t="shared" ref="D3:D18" si="1">AVERAGE(3*E3,F3,G3,H3,I3)</f>
-        <v>1.8</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E3" s="83">
         <f>POINTS!H22</f>
@@ -6734,11 +6734,11 @@
       </c>
       <c r="H3" s="83">
         <f>POINTS!K22</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I3" s="84">
         <f>POINTS!L22</f>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="J3" s="78"/>
     </row>
@@ -6749,11 +6749,11 @@
       </c>
       <c r="C4" s="71">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D4" s="85">
         <f t="shared" si="1"/>
-        <v>12.8</v>
+        <v>15.2</v>
       </c>
       <c r="E4" s="86">
         <f>POINTS!H23</f>
@@ -6773,7 +6773,7 @@
       </c>
       <c r="I4" s="87">
         <f>POINTS!L23</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J4" s="79"/>
     </row>
@@ -6788,7 +6788,7 @@
       </c>
       <c r="D5" s="85">
         <f t="shared" si="1"/>
-        <v>19.2</v>
+        <v>20</v>
       </c>
       <c r="E5" s="86">
         <f>POINTS!H24</f>
@@ -6808,7 +6808,7 @@
       </c>
       <c r="I5" s="87">
         <f>POINTS!L24</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J5" s="79"/>
     </row>
@@ -6819,11 +6819,11 @@
       </c>
       <c r="C6" s="71">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" s="85">
         <f t="shared" si="1"/>
-        <v>12.8</v>
+        <v>14.2</v>
       </c>
       <c r="E6" s="86">
         <f>POINTS!H25</f>
@@ -6831,19 +6831,19 @@
       </c>
       <c r="F6" s="86">
         <f>POINTS!I25</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G6" s="86">
         <f>POINTS!J25</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H6" s="86">
         <f>POINTS!K25</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I6" s="87">
         <f>POINTS!L25</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J6" s="79"/>
     </row>
@@ -6854,31 +6854,31 @@
       </c>
       <c r="C7" s="71">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" s="85">
         <f t="shared" si="1"/>
-        <v>14.6</v>
+        <v>17</v>
       </c>
       <c r="E7" s="86">
         <f>POINTS!H26</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F7" s="86">
         <f>POINTS!I26</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G7" s="86">
         <f>POINTS!J26</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7" s="86">
         <f>POINTS!K26</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I7" s="87">
         <f>POINTS!L26</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J7" s="79"/>
     </row>
@@ -6889,31 +6889,31 @@
       </c>
       <c r="C8" s="71">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D8" s="85">
         <f t="shared" si="1"/>
-        <v>6.8</v>
+        <v>11</v>
       </c>
       <c r="E8" s="86">
         <f>POINTS!H27</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F8" s="86">
         <f>POINTS!I27</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G8" s="86">
         <f>POINTS!J27</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H8" s="86">
         <f>POINTS!K27</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I8" s="87">
         <f>POINTS!L27</f>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="J8" s="79"/>
     </row>
@@ -6928,7 +6928,7 @@
       </c>
       <c r="D9" s="85">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6.8</v>
       </c>
       <c r="E9" s="86">
         <f>POINTS!H28</f>
@@ -6944,11 +6944,11 @@
       </c>
       <c r="H9" s="86">
         <f>POINTS!K28</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I9" s="87">
         <f>POINTS!L28</f>
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="J9" s="79"/>
     </row>
@@ -6959,15 +6959,15 @@
       </c>
       <c r="C10" s="71">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" s="85">
         <f t="shared" si="1"/>
-        <v>9.6</v>
+        <v>10.4</v>
       </c>
       <c r="E10" s="86">
         <f>POINTS!H29</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F10" s="86">
         <f>POINTS!I29</f>
@@ -6983,7 +6983,7 @@
       </c>
       <c r="I10" s="87">
         <f>POINTS!L29</f>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="J10" s="79"/>
     </row>
@@ -6998,7 +6998,7 @@
       </c>
       <c r="D11" s="85">
         <f t="shared" si="1"/>
-        <v>13.4</v>
+        <v>14.6</v>
       </c>
       <c r="E11" s="86">
         <f>POINTS!H30</f>
@@ -7010,15 +7010,15 @@
       </c>
       <c r="G11" s="86">
         <f>POINTS!J30</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H11" s="86">
         <f>POINTS!K30</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I11" s="87">
         <f>POINTS!L30</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J11" s="79"/>
     </row>
@@ -7029,31 +7029,31 @@
       </c>
       <c r="C12" s="71">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="85">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E12" s="86">
         <f>POINTS!H31</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12" s="86">
         <f>POINTS!I31</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" s="86">
         <f>POINTS!J31</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H12" s="86">
         <f>POINTS!K31</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I12" s="87">
         <f>POINTS!L31</f>
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="J12" s="79"/>
     </row>
@@ -7064,11 +7064,11 @@
       </c>
       <c r="C13" s="71">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D13" s="85">
         <f t="shared" si="1"/>
-        <v>8.4</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="E13" s="86">
         <f>POINTS!H32</f>
@@ -7088,7 +7088,7 @@
       </c>
       <c r="I13" s="87">
         <f>POINTS!L32</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J13" s="79"/>
     </row>
@@ -7103,7 +7103,7 @@
       </c>
       <c r="D14" s="85">
         <f t="shared" si="1"/>
-        <v>2.6</v>
+        <v>5.4</v>
       </c>
       <c r="E14" s="86">
         <f>POINTS!H33</f>
@@ -7123,7 +7123,7 @@
       </c>
       <c r="I14" s="87">
         <f>POINTS!L33</f>
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="J14" s="79"/>
     </row>
@@ -7134,23 +7134,23 @@
       </c>
       <c r="C15" s="71">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D15" s="85">
         <f t="shared" si="1"/>
-        <v>13.4</v>
+        <v>12.8</v>
       </c>
       <c r="E15" s="86">
         <f>POINTS!H34</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F15" s="86">
         <f>POINTS!I34</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G15" s="86">
         <f>POINTS!J34</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H15" s="86">
         <f>POINTS!K34</f>
@@ -7158,7 +7158,7 @@
       </c>
       <c r="I15" s="87">
         <f>POINTS!L34</f>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="J15" s="79"/>
     </row>
@@ -7173,7 +7173,7 @@
       </c>
       <c r="D16" s="85">
         <f t="shared" si="1"/>
-        <v>8.1999999999999993</v>
+        <v>9</v>
       </c>
       <c r="E16" s="86">
         <f>POINTS!H35</f>
@@ -7181,19 +7181,19 @@
       </c>
       <c r="F16" s="86">
         <f>POINTS!I35</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G16" s="86">
         <f>POINTS!J35</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H16" s="86">
         <f>POINTS!K35</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I16" s="87">
         <f>POINTS!L35</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J16" s="79"/>
     </row>
@@ -7285,7 +7285,7 @@
   <dimension ref="B2:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B3" sqref="B3:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -7338,7 +7338,7 @@
       </c>
       <c r="D3" s="82">
         <f>AVERAGE(3*E3,F3,G3,H3,I3)</f>
-        <v>1.8</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E3" s="83">
         <f>POINTS!H22</f>
@@ -7354,11 +7354,11 @@
       </c>
       <c r="H3" s="83">
         <f>POINTS!K22</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I3" s="84">
         <f>POINTS!L22</f>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="J3" s="78"/>
     </row>
@@ -7373,7 +7373,7 @@
       </c>
       <c r="D4" s="85">
         <f>AVERAGE(3*E4,F4,G4,H4,I4)</f>
-        <v>2.6</v>
+        <v>5.4</v>
       </c>
       <c r="E4" s="86">
         <f>POINTS!H33</f>
@@ -7393,7 +7393,7 @@
       </c>
       <c r="I4" s="87">
         <f>POINTS!L33</f>
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="J4" s="79"/>
     </row>
@@ -7408,7 +7408,7 @@
       </c>
       <c r="D5" s="85">
         <f>AVERAGE(3*E5,F5,G5,H5,I5)</f>
-        <v>4</v>
+        <v>6.8</v>
       </c>
       <c r="E5" s="86">
         <f>POINTS!H28</f>
@@ -7424,18 +7424,18 @@
       </c>
       <c r="H5" s="86">
         <f>POINTS!K28</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I5" s="87">
         <f>POINTS!L28</f>
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="J5" s="79"/>
     </row>
     <row r="6" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B6" s="92" t="str">
-        <f>POINTS!B8</f>
-        <v>Deflate Deez Nutz</v>
+        <f>POINTS!B13</f>
+        <v>OhNo Romo</v>
       </c>
       <c r="C6" s="71">
         <f>RANK(D6,$D$3:$D$16,1)</f>
@@ -7443,27 +7443,27 @@
       </c>
       <c r="D6" s="85">
         <f>AVERAGE(3*E6,F6,G6,H6,I6)</f>
-        <v>6.8</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="E6" s="86">
-        <f>POINTS!H27</f>
+        <f>POINTS!H32</f>
         <v>4</v>
       </c>
       <c r="F6" s="86">
-        <f>POINTS!I27</f>
+        <f>POINTS!I32</f>
+        <v>6</v>
+      </c>
+      <c r="G6" s="86">
+        <f>POINTS!J32</f>
         <v>5</v>
       </c>
-      <c r="G6" s="86">
-        <f>POINTS!J27</f>
-        <v>6</v>
-      </c>
       <c r="H6" s="86">
-        <f>POINTS!K27</f>
-        <v>6</v>
+        <f>POINTS!K32</f>
+        <v>5</v>
       </c>
       <c r="I6" s="87">
-        <f>POINTS!L27</f>
-        <v>5</v>
+        <f>POINTS!L32</f>
+        <v>16</v>
       </c>
       <c r="J6" s="79"/>
     </row>
@@ -7478,7 +7478,7 @@
       </c>
       <c r="D7" s="85">
         <f>AVERAGE(3*E7,F7,G7,H7,I7)</f>
-        <v>8.1999999999999993</v>
+        <v>9</v>
       </c>
       <c r="E7" s="86">
         <f>POINTS!H35</f>
@@ -7486,26 +7486,26 @@
       </c>
       <c r="F7" s="86">
         <f>POINTS!I35</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G7" s="86">
         <f>POINTS!J35</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H7" s="86">
         <f>POINTS!K35</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I7" s="87">
         <f>POINTS!L35</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J7" s="79"/>
     </row>
     <row r="8" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B8" s="92" t="str">
-        <f>POINTS!B13</f>
-        <v>OhNo Romo</v>
+        <f>POINTS!B10</f>
+        <v>Team Wasserman</v>
       </c>
       <c r="C8" s="71">
         <f>RANK(D8,$D$3:$D$16,1)</f>
@@ -7513,34 +7513,34 @@
       </c>
       <c r="D8" s="85">
         <f>AVERAGE(3*E8,F8,G8,H8,I8)</f>
-        <v>8.4</v>
+        <v>10.4</v>
       </c>
       <c r="E8" s="86">
-        <f>POINTS!H32</f>
+        <f>POINTS!H29</f>
+        <v>8</v>
+      </c>
+      <c r="F8" s="86">
+        <f>POINTS!I29</f>
         <v>4</v>
       </c>
-      <c r="F8" s="86">
-        <f>POINTS!I32</f>
-        <v>6</v>
-      </c>
       <c r="G8" s="86">
-        <f>POINTS!J32</f>
-        <v>5</v>
+        <f>POINTS!J29</f>
+        <v>4</v>
       </c>
       <c r="H8" s="86">
-        <f>POINTS!K32</f>
-        <v>5</v>
+        <f>POINTS!K29</f>
+        <v>4</v>
       </c>
       <c r="I8" s="87">
-        <f>POINTS!L32</f>
-        <v>14</v>
+        <f>POINTS!L29</f>
+        <v>16</v>
       </c>
       <c r="J8" s="79"/>
     </row>
     <row r="9" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B9" s="92" t="str">
-        <f>POINTS!B10</f>
-        <v>Team Wasserman</v>
+        <f>POINTS!B8</f>
+        <v>Deflate Deez Nutz</v>
       </c>
       <c r="C9" s="71">
         <f>RANK(D9,$D$3:$D$16,1)</f>
@@ -7548,34 +7548,34 @@
       </c>
       <c r="D9" s="85">
         <f>AVERAGE(3*E9,F9,G9,H9,I9)</f>
-        <v>9.6</v>
+        <v>11</v>
       </c>
       <c r="E9" s="86">
-        <f>POINTS!H29</f>
-        <v>10</v>
+        <f>POINTS!H27</f>
+        <v>6</v>
       </c>
       <c r="F9" s="86">
-        <f>POINTS!I29</f>
-        <v>4</v>
+        <f>POINTS!I27</f>
+        <v>7</v>
       </c>
       <c r="G9" s="86">
-        <f>POINTS!J29</f>
-        <v>4</v>
+        <f>POINTS!J27</f>
+        <v>7</v>
       </c>
       <c r="H9" s="86">
-        <f>POINTS!K29</f>
-        <v>4</v>
+        <f>POINTS!K27</f>
+        <v>7</v>
       </c>
       <c r="I9" s="87">
-        <f>POINTS!L29</f>
-        <v>6</v>
+        <f>POINTS!L27</f>
+        <v>16</v>
       </c>
       <c r="J9" s="79"/>
     </row>
     <row r="10" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B10" s="92" t="str">
-        <f>POINTS!B6</f>
-        <v>Team Thomas</v>
+        <f>POINTS!B15</f>
+        <v>Hebrew Wolves</v>
       </c>
       <c r="C10" s="71">
         <f>RANK(D10,$D$3:$D$16,1)</f>
@@ -7586,59 +7586,59 @@
         <v>12.8</v>
       </c>
       <c r="E10" s="86">
+        <f>POINTS!H34</f>
+        <v>8</v>
+      </c>
+      <c r="F10" s="86">
+        <f>POINTS!I34</f>
+        <v>8</v>
+      </c>
+      <c r="G10" s="86">
+        <f>POINTS!J34</f>
+        <v>8</v>
+      </c>
+      <c r="H10" s="86">
+        <f>POINTS!K34</f>
+        <v>8</v>
+      </c>
+      <c r="I10" s="87">
+        <f>POINTS!L34</f>
+        <v>16</v>
+      </c>
+      <c r="J10" s="79"/>
+    </row>
+    <row r="11" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B11" s="92" t="str">
+        <f>POINTS!B6</f>
+        <v>Team Thomas</v>
+      </c>
+      <c r="C11" s="71">
+        <f>RANK(D11,$D$3:$D$16,1)</f>
+        <v>9</v>
+      </c>
+      <c r="D11" s="85">
+        <f>AVERAGE(3*E11,F11,G11,H11,I11)</f>
+        <v>14.2</v>
+      </c>
+      <c r="E11" s="86">
         <f>POINTS!H25</f>
         <v>8</v>
       </c>
-      <c r="F10" s="86">
+      <c r="F11" s="86">
         <f>POINTS!I25</f>
-        <v>8</v>
-      </c>
-      <c r="G10" s="86">
+        <v>9</v>
+      </c>
+      <c r="G11" s="86">
         <f>POINTS!J25</f>
+        <v>12</v>
+      </c>
+      <c r="H11" s="86">
+        <f>POINTS!K25</f>
         <v>10</v>
       </c>
-      <c r="H10" s="86">
-        <f>POINTS!K25</f>
-        <v>9</v>
-      </c>
-      <c r="I10" s="87">
+      <c r="I11" s="87">
         <f>POINTS!L25</f>
-        <v>13</v>
-      </c>
-      <c r="J10" s="79"/>
-    </row>
-    <row r="11" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B11" s="92" t="str">
-        <f>POINTS!B4</f>
-        <v>Little Miss Moffet</v>
-      </c>
-      <c r="C11" s="71">
-        <f>RANK(D11,$D$3:$D$16,1)</f>
-        <v>8</v>
-      </c>
-      <c r="D11" s="85">
-        <f>AVERAGE(3*E11,F11,G11,H11,I11)</f>
-        <v>12.8</v>
-      </c>
-      <c r="E11" s="86">
-        <f>POINTS!H23</f>
-        <v>7</v>
-      </c>
-      <c r="F11" s="86">
-        <f>POINTS!I23</f>
-        <v>13</v>
-      </c>
-      <c r="G11" s="86">
-        <f>POINTS!J23</f>
-        <v>13</v>
-      </c>
-      <c r="H11" s="86">
-        <f>POINTS!K23</f>
-        <v>13</v>
-      </c>
-      <c r="I11" s="87">
-        <f>POINTS!L23</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J11" s="79"/>
     </row>
@@ -7653,7 +7653,7 @@
       </c>
       <c r="D12" s="85">
         <f>AVERAGE(3*E12,F12,G12,H12,I12)</f>
-        <v>13.4</v>
+        <v>14.6</v>
       </c>
       <c r="E12" s="86">
         <f>POINTS!H30</f>
@@ -7665,57 +7665,57 @@
       </c>
       <c r="G12" s="86">
         <f>POINTS!J30</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H12" s="86">
         <f>POINTS!K30</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I12" s="87">
         <f>POINTS!L30</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J12" s="79"/>
     </row>
     <row r="13" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B13" s="92" t="str">
-        <f>POINTS!B15</f>
-        <v>Hebrew Wolves</v>
+        <f>POINTS!B4</f>
+        <v>Little Miss Moffet</v>
       </c>
       <c r="C13" s="71">
         <f>RANK(D13,$D$3:$D$16,1)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D13" s="85">
         <f>AVERAGE(3*E13,F13,G13,H13,I13)</f>
-        <v>13.4</v>
+        <v>15.2</v>
       </c>
       <c r="E13" s="86">
-        <f>POINTS!H34</f>
-        <v>10</v>
+        <f>POINTS!H23</f>
+        <v>7</v>
       </c>
       <c r="F13" s="86">
-        <f>POINTS!I34</f>
-        <v>9</v>
+        <f>POINTS!I23</f>
+        <v>13</v>
       </c>
       <c r="G13" s="86">
-        <f>POINTS!J34</f>
-        <v>11</v>
+        <f>POINTS!J23</f>
+        <v>13</v>
       </c>
       <c r="H13" s="86">
-        <f>POINTS!K34</f>
-        <v>8</v>
+        <f>POINTS!K23</f>
+        <v>13</v>
       </c>
       <c r="I13" s="87">
-        <f>POINTS!L34</f>
-        <v>9</v>
+        <f>POINTS!L23</f>
+        <v>16</v>
       </c>
       <c r="J13" s="79"/>
     </row>
     <row r="14" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B14" s="92" t="str">
-        <f>POINTS!B7</f>
-        <v>Gurley Gone Wild</v>
+        <f>POINTS!B12</f>
+        <v>Team Frisch</v>
       </c>
       <c r="C14" s="71">
         <f>RANK(D14,$D$3:$D$16,1)</f>
@@ -7723,34 +7723,34 @@
       </c>
       <c r="D14" s="85">
         <f>AVERAGE(3*E14,F14,G14,H14,I14)</f>
-        <v>14.6</v>
+        <v>16</v>
       </c>
       <c r="E14" s="86">
-        <f>POINTS!H26</f>
+        <f>POINTS!H31</f>
+        <v>12</v>
+      </c>
+      <c r="F14" s="86">
+        <f>POINTS!I31</f>
         <v>10</v>
       </c>
-      <c r="F14" s="86">
-        <f>POINTS!I26</f>
+      <c r="G14" s="86">
+        <f>POINTS!J31</f>
         <v>9</v>
       </c>
-      <c r="G14" s="86">
-        <f>POINTS!J26</f>
-        <v>12</v>
-      </c>
       <c r="H14" s="86">
-        <f>POINTS!K26</f>
-        <v>11</v>
+        <f>POINTS!K31</f>
+        <v>9</v>
       </c>
       <c r="I14" s="87">
-        <f>POINTS!L26</f>
-        <v>11</v>
+        <f>POINTS!L31</f>
+        <v>16</v>
       </c>
       <c r="J14" s="79"/>
     </row>
     <row r="15" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B15" s="92" t="str">
-        <f>POINTS!B12</f>
-        <v>Team Frisch</v>
+        <f>POINTS!B7</f>
+        <v>Gurley Gone Wild</v>
       </c>
       <c r="C15" s="71">
         <f>RANK(D15,$D$3:$D$16,1)</f>
@@ -7758,27 +7758,27 @@
       </c>
       <c r="D15" s="85">
         <f>AVERAGE(3*E15,F15,G15,H15,I15)</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E15" s="86">
-        <f>POINTS!H31</f>
-        <v>13</v>
+        <f>POINTS!H26</f>
+        <v>12</v>
       </c>
       <c r="F15" s="86">
-        <f>POINTS!I31</f>
+        <f>POINTS!I26</f>
+        <v>10</v>
+      </c>
+      <c r="G15" s="86">
+        <f>POINTS!J26</f>
         <v>11</v>
       </c>
-      <c r="G15" s="86">
-        <f>POINTS!J31</f>
-        <v>8</v>
-      </c>
       <c r="H15" s="86">
-        <f>POINTS!K31</f>
-        <v>10</v>
+        <f>POINTS!K26</f>
+        <v>12</v>
       </c>
       <c r="I15" s="87">
-        <f>POINTS!L31</f>
-        <v>7</v>
+        <f>POINTS!L26</f>
+        <v>16</v>
       </c>
       <c r="J15" s="79"/>
     </row>
@@ -7793,7 +7793,7 @@
       </c>
       <c r="D16" s="88">
         <f>AVERAGE(3*E16,F16,G16,H16,I16)</f>
-        <v>19.2</v>
+        <v>20</v>
       </c>
       <c r="E16" s="89">
         <f>POINTS!H24</f>
@@ -7813,7 +7813,7 @@
       </c>
       <c r="I16" s="90">
         <f>POINTS!L24</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J16" s="80"/>
     </row>
@@ -7885,7 +7885,7 @@
       </c>
       <c r="D3" s="82">
         <f t="shared" ref="D3:D14" si="1">AVERAGE(3*E3,F3,G3,H3,I3)</f>
-        <v>1.8</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E3" s="83">
         <f>POINTS!H22</f>
@@ -7901,11 +7901,11 @@
       </c>
       <c r="H3" s="83">
         <f>POINTS!K22</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I3" s="84">
         <f>POINTS!L22</f>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="J3" s="78"/>
     </row>
@@ -7916,11 +7916,11 @@
       </c>
       <c r="C4" s="71">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" s="85">
         <f t="shared" si="1"/>
-        <v>12.8</v>
+        <v>15.2</v>
       </c>
       <c r="E4" s="86">
         <f>POINTS!H23</f>
@@ -7940,7 +7940,7 @@
       </c>
       <c r="I4" s="87">
         <f>POINTS!L23</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J4" s="79"/>
     </row>
@@ -7955,7 +7955,7 @@
       </c>
       <c r="D5" s="85">
         <f t="shared" si="1"/>
-        <v>19.2</v>
+        <v>20</v>
       </c>
       <c r="E5" s="86">
         <f>POINTS!H24</f>
@@ -7975,7 +7975,7 @@
       </c>
       <c r="I5" s="87">
         <f>POINTS!L24</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J5" s="79"/>
     </row>
@@ -7990,7 +7990,7 @@
       </c>
       <c r="D6" s="85">
         <f t="shared" si="1"/>
-        <v>12.8</v>
+        <v>14.2</v>
       </c>
       <c r="E6" s="86">
         <f>POINTS!H25</f>
@@ -7998,19 +7998,19 @@
       </c>
       <c r="F6" s="86">
         <f>POINTS!I25</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G6" s="86">
         <f>POINTS!J25</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H6" s="86">
         <f>POINTS!K25</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I6" s="87">
         <f>POINTS!L25</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J6" s="79"/>
     </row>
@@ -8021,31 +8021,31 @@
       </c>
       <c r="C7" s="71">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" s="85">
         <f t="shared" si="1"/>
-        <v>14.6</v>
+        <v>17</v>
       </c>
       <c r="E7" s="86">
         <f>POINTS!H26</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F7" s="86">
         <f>POINTS!I26</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G7" s="86">
         <f>POINTS!J26</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7" s="86">
         <f>POINTS!K26</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I7" s="87">
         <f>POINTS!L26</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J7" s="79"/>
     </row>
@@ -8056,31 +8056,31 @@
       </c>
       <c r="C8" s="71">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D8" s="85">
         <f t="shared" si="1"/>
-        <v>6.8</v>
+        <v>11</v>
       </c>
       <c r="E8" s="86">
         <f>POINTS!H27</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F8" s="86">
         <f>POINTS!I27</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G8" s="86">
         <f>POINTS!J27</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H8" s="86">
         <f>POINTS!K27</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I8" s="87">
         <f>POINTS!L27</f>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="J8" s="79"/>
     </row>
@@ -8095,7 +8095,7 @@
       </c>
       <c r="D9" s="85">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6.8</v>
       </c>
       <c r="E9" s="86">
         <f>POINTS!H28</f>
@@ -8111,11 +8111,11 @@
       </c>
       <c r="H9" s="86">
         <f>POINTS!K28</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I9" s="87">
         <f>POINTS!L28</f>
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="J9" s="79"/>
     </row>
@@ -8126,15 +8126,15 @@
       </c>
       <c r="C10" s="71">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="85">
         <f t="shared" si="1"/>
-        <v>9.6</v>
+        <v>10.4</v>
       </c>
       <c r="E10" s="86">
         <f>POINTS!H29</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F10" s="86">
         <f>POINTS!I29</f>
@@ -8150,7 +8150,7 @@
       </c>
       <c r="I10" s="87">
         <f>POINTS!L29</f>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="J10" s="79"/>
     </row>
@@ -8161,11 +8161,11 @@
       </c>
       <c r="C11" s="71">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="85">
         <f t="shared" si="1"/>
-        <v>13.4</v>
+        <v>14.6</v>
       </c>
       <c r="E11" s="86">
         <f>POINTS!H30</f>
@@ -8177,15 +8177,15 @@
       </c>
       <c r="G11" s="86">
         <f>POINTS!J30</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H11" s="86">
         <f>POINTS!K30</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I11" s="87">
         <f>POINTS!L30</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J11" s="79"/>
     </row>
@@ -8196,31 +8196,31 @@
       </c>
       <c r="C12" s="71">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="85">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E12" s="86">
         <f>POINTS!H31</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12" s="86">
         <f>POINTS!I31</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" s="86">
         <f>POINTS!J31</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H12" s="86">
         <f>POINTS!K31</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I12" s="87">
         <f>POINTS!L31</f>
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="J12" s="79"/>
     </row>
@@ -8231,11 +8231,11 @@
       </c>
       <c r="C13" s="71">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" s="85">
         <f t="shared" si="1"/>
-        <v>8.4</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="E13" s="86">
         <f>POINTS!H32</f>
@@ -8255,7 +8255,7 @@
       </c>
       <c r="I13" s="87">
         <f>POINTS!L32</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J13" s="79"/>
     </row>
@@ -8270,7 +8270,7 @@
       </c>
       <c r="D14" s="88">
         <f t="shared" si="1"/>
-        <v>2.6</v>
+        <v>5.4</v>
       </c>
       <c r="E14" s="89">
         <f>POINTS!H33</f>
@@ -8290,7 +8290,7 @@
       </c>
       <c r="I14" s="90">
         <f>POINTS!L33</f>
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="J14" s="80"/>
     </row>
@@ -8362,7 +8362,7 @@
       </c>
       <c r="D3" s="83">
         <f t="shared" ref="D3:D12" si="1">AVERAGE(3*E3,F3,G3,H3,I3)</f>
-        <v>1.8</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E3" s="83">
         <f>POINTS!H22</f>
@@ -8378,11 +8378,11 @@
       </c>
       <c r="H3" s="83">
         <f>POINTS!K22</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I3" s="83">
         <f>POINTS!L22</f>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="J3" s="73"/>
     </row>
@@ -8393,11 +8393,11 @@
       </c>
       <c r="C4" s="97">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D4" s="86">
         <f t="shared" si="1"/>
-        <v>12.8</v>
+        <v>15.2</v>
       </c>
       <c r="E4" s="86">
         <f>POINTS!H23</f>
@@ -8417,7 +8417,7 @@
       </c>
       <c r="I4" s="86">
         <f>POINTS!L23</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J4" s="74"/>
     </row>
@@ -8432,7 +8432,7 @@
       </c>
       <c r="D5" s="86">
         <f t="shared" si="1"/>
-        <v>19.2</v>
+        <v>20</v>
       </c>
       <c r="E5" s="86">
         <f>POINTS!H24</f>
@@ -8452,7 +8452,7 @@
       </c>
       <c r="I5" s="86">
         <f>POINTS!L24</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J5" s="74"/>
     </row>
@@ -8467,7 +8467,7 @@
       </c>
       <c r="D6" s="86">
         <f t="shared" si="1"/>
-        <v>12.8</v>
+        <v>14.2</v>
       </c>
       <c r="E6" s="86">
         <f>POINTS!H25</f>
@@ -8475,19 +8475,19 @@
       </c>
       <c r="F6" s="86">
         <f>POINTS!I25</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G6" s="86">
         <f>POINTS!J25</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H6" s="86">
         <f>POINTS!K25</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I6" s="86">
         <f>POINTS!L25</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J6" s="74"/>
     </row>
@@ -8498,31 +8498,31 @@
       </c>
       <c r="C7" s="97">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" s="86">
         <f t="shared" si="1"/>
-        <v>14.6</v>
+        <v>17</v>
       </c>
       <c r="E7" s="86">
         <f>POINTS!H26</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F7" s="86">
         <f>POINTS!I26</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G7" s="86">
         <f>POINTS!J26</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7" s="86">
         <f>POINTS!K26</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I7" s="86">
         <f>POINTS!L26</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J7" s="74"/>
     </row>
@@ -8533,31 +8533,31 @@
       </c>
       <c r="C8" s="97">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8" s="86">
         <f t="shared" si="1"/>
-        <v>6.8</v>
+        <v>11</v>
       </c>
       <c r="E8" s="86">
         <f>POINTS!H27</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F8" s="86">
         <f>POINTS!I27</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G8" s="86">
         <f>POINTS!J27</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H8" s="86">
         <f>POINTS!K27</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I8" s="86">
         <f>POINTS!L27</f>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="J8" s="74"/>
     </row>
@@ -8572,7 +8572,7 @@
       </c>
       <c r="D9" s="86">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6.8</v>
       </c>
       <c r="E9" s="86">
         <f>POINTS!H28</f>
@@ -8588,11 +8588,11 @@
       </c>
       <c r="H9" s="86">
         <f>POINTS!K28</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I9" s="86">
         <f>POINTS!L28</f>
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="J9" s="74"/>
     </row>
@@ -8603,15 +8603,15 @@
       </c>
       <c r="C10" s="97">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="86">
         <f t="shared" si="1"/>
-        <v>9.6</v>
+        <v>10.4</v>
       </c>
       <c r="E10" s="86">
         <f>POINTS!H29</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F10" s="86">
         <f>POINTS!I29</f>
@@ -8627,7 +8627,7 @@
       </c>
       <c r="I10" s="86">
         <f>POINTS!L29</f>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="J10" s="74"/>
     </row>
@@ -8638,11 +8638,11 @@
       </c>
       <c r="C11" s="97">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" s="86">
         <f t="shared" si="1"/>
-        <v>13.4</v>
+        <v>14.6</v>
       </c>
       <c r="E11" s="86">
         <f>POINTS!H30</f>
@@ -8654,15 +8654,15 @@
       </c>
       <c r="G11" s="86">
         <f>POINTS!J30</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H11" s="86">
         <f>POINTS!K30</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I11" s="86">
         <f>POINTS!L30</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J11" s="74"/>
     </row>
@@ -8673,31 +8673,31 @@
       </c>
       <c r="C12" s="99">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12" s="89">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E12" s="89">
         <f>POINTS!H31</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12" s="89">
         <f>POINTS!I31</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" s="89">
         <f>POINTS!J31</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H12" s="89">
         <f>POINTS!K31</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I12" s="89">
         <f>POINTS!L31</f>
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="J12" s="75"/>
     </row>
@@ -8769,7 +8769,7 @@
       </c>
       <c r="D3" s="82">
         <f t="shared" ref="D3:D10" si="1">AVERAGE(3*E3,F3,G3,H3,I3)</f>
-        <v>1.8</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E3" s="83">
         <f>POINTS!H22</f>
@@ -8785,11 +8785,11 @@
       </c>
       <c r="H3" s="83">
         <f>POINTS!K22</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I3" s="84">
         <f>POINTS!L22</f>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="J3" s="78"/>
     </row>
@@ -8800,11 +8800,11 @@
       </c>
       <c r="C4" s="71">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4" s="85">
         <f t="shared" si="1"/>
-        <v>12.8</v>
+        <v>15.2</v>
       </c>
       <c r="E4" s="86">
         <f>POINTS!H23</f>
@@ -8824,7 +8824,7 @@
       </c>
       <c r="I4" s="87">
         <f>POINTS!L23</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J4" s="79"/>
     </row>
@@ -8839,7 +8839,7 @@
       </c>
       <c r="D5" s="85">
         <f t="shared" si="1"/>
-        <v>19.2</v>
+        <v>20</v>
       </c>
       <c r="E5" s="86">
         <f>POINTS!H24</f>
@@ -8859,7 +8859,7 @@
       </c>
       <c r="I5" s="87">
         <f>POINTS!L24</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J5" s="79"/>
     </row>
@@ -8874,7 +8874,7 @@
       </c>
       <c r="D6" s="85">
         <f t="shared" si="1"/>
-        <v>12.8</v>
+        <v>14.2</v>
       </c>
       <c r="E6" s="86">
         <f>POINTS!H25</f>
@@ -8882,19 +8882,19 @@
       </c>
       <c r="F6" s="86">
         <f>POINTS!I25</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G6" s="86">
         <f>POINTS!J25</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H6" s="86">
         <f>POINTS!K25</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I6" s="87">
         <f>POINTS!L25</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J6" s="79"/>
     </row>
@@ -8909,27 +8909,27 @@
       </c>
       <c r="D7" s="85">
         <f t="shared" si="1"/>
-        <v>14.6</v>
+        <v>17</v>
       </c>
       <c r="E7" s="86">
         <f>POINTS!H26</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F7" s="86">
         <f>POINTS!I26</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G7" s="86">
         <f>POINTS!J26</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7" s="86">
         <f>POINTS!K26</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I7" s="87">
         <f>POINTS!L26</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J7" s="79"/>
     </row>
@@ -8940,31 +8940,31 @@
       </c>
       <c r="C8" s="71">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8" s="85">
         <f t="shared" si="1"/>
-        <v>6.8</v>
+        <v>11</v>
       </c>
       <c r="E8" s="86">
         <f>POINTS!H27</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F8" s="86">
         <f>POINTS!I27</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G8" s="86">
         <f>POINTS!J27</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H8" s="86">
         <f>POINTS!K27</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I8" s="87">
         <f>POINTS!L27</f>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="J8" s="79"/>
     </row>
@@ -8979,7 +8979,7 @@
       </c>
       <c r="D9" s="85">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6.8</v>
       </c>
       <c r="E9" s="86">
         <f>POINTS!H28</f>
@@ -8995,11 +8995,11 @@
       </c>
       <c r="H9" s="86">
         <f>POINTS!K28</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I9" s="87">
         <f>POINTS!L28</f>
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="J9" s="79"/>
     </row>
@@ -9010,15 +9010,15 @@
       </c>
       <c r="C10" s="72">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="88">
         <f t="shared" si="1"/>
-        <v>9.6</v>
+        <v>10.4</v>
       </c>
       <c r="E10" s="89">
         <f>POINTS!H29</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F10" s="89">
         <f>POINTS!I29</f>
@@ -9034,7 +9034,7 @@
       </c>
       <c r="I10" s="90">
         <f>POINTS!L29</f>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="J10" s="80"/>
     </row>

</xml_diff>